<commit_message>
TS 7 Kramam files conv to Docx. - 22/03/2022
</commit_message>
<xml_diff>
--- a/Ghana Maala/Ghana Maala Content.xlsx
+++ b/Ghana Maala/Ghana Maala Content.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\Ghana Maala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982DCC00-7DCC-4BB6-AD0E-EB3A7C4AA0DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563772E5-8E84-43D2-A5A2-2429EEC005CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$2:$F$85</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1451,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ghana Malaa Corrections incl Ghanam files - 27072022
</commit_message>
<xml_diff>
--- a/Ghana Maala/Ghana Maala Content.xlsx
+++ b/Ghana Maala/Ghana Maala Content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\Ghana Maala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A81EF66-D340-4D37-8A09-5181B4391E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB34DF3-E892-47B2-8E32-248388CE0CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -980,7 +980,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -998,6 +998,12 @@
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1101,7 +1107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1121,9 +1127,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1171,6 +1174,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1512,14 +1524,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="18" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
@@ -1529,7 +1541,7 @@
   <sheetData>
     <row r="2" spans="1:7" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>105</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1552,7 +1564,7 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>115</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1574,7 +1586,7 @@
         <f>+A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>116</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1583,7 +1595,7 @@
       <c r="D4" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="6" t="s">
         <v>216</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -1596,7 +1608,7 @@
         <f t="shared" ref="A5:A110" si="0">+A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>117</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1618,7 +1630,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1.4</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1640,7 +1652,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>1.5</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1662,7 +1674,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>1.6</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1684,7 +1696,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>1.7</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1706,7 +1718,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>1.8</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1728,7 +1740,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>1.9</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1750,7 +1762,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>118</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1772,7 +1784,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>119</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1781,10 +1793,10 @@
       <c r="D13" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>171</v>
       </c>
       <c r="G13" s="3"/>
@@ -1794,7 +1806,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>120</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1816,7 +1828,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>121</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1838,7 +1850,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>281</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1860,7 +1872,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>122</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1869,7 +1881,7 @@
       <c r="D17" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="6" t="s">
         <v>224</v>
       </c>
       <c r="F17" s="7" t="s">
@@ -1882,7 +1894,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>1.1599999999999999</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1891,10 +1903,10 @@
       <c r="D18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="13" t="s">
         <v>169</v>
       </c>
       <c r="G18" s="3"/>
@@ -1904,7 +1916,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>125</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1913,7 +1925,7 @@
       <c r="D19" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="6" t="s">
         <v>225</v>
       </c>
       <c r="F19" s="7" t="s">
@@ -1926,7 +1938,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>124</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1938,7 +1950,7 @@
       <c r="E20" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="12" t="s">
         <v>177</v>
       </c>
       <c r="G20" s="3"/>
@@ -1948,7 +1960,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>123</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1960,7 +1972,7 @@
       <c r="E21" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="11" t="s">
         <v>62</v>
       </c>
       <c r="G21" s="3"/>
@@ -1970,7 +1982,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>127</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1982,7 +1994,7 @@
       <c r="E22" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="11" t="s">
         <v>63</v>
       </c>
       <c r="G22" s="3"/>
@@ -1992,7 +2004,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>128</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -2004,7 +2016,7 @@
       <c r="E23" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="11" t="s">
         <v>24</v>
       </c>
       <c r="G23" s="3"/>
@@ -2014,7 +2026,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>135</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -2026,7 +2038,7 @@
       <c r="E24" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="11" t="s">
         <v>60</v>
       </c>
       <c r="G24" s="3"/>
@@ -2036,7 +2048,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>126</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -2048,7 +2060,7 @@
       <c r="E25" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="11" t="s">
         <v>30</v>
       </c>
       <c r="G25" s="3"/>
@@ -2058,7 +2070,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>138</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -2067,10 +2079,10 @@
       <c r="D26" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G26" s="3"/>
@@ -2080,7 +2092,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>129</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2092,7 +2104,7 @@
       <c r="E27" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="F27" s="11" t="s">
         <v>49</v>
       </c>
       <c r="G27" s="3"/>
@@ -2102,7 +2114,7 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>130</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2114,7 +2126,7 @@
       <c r="E28" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="11" t="s">
         <v>50</v>
       </c>
       <c r="G28" s="3"/>
@@ -2124,7 +2136,7 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>133</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -2136,7 +2148,7 @@
       <c r="E29" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="F29" s="11" t="s">
         <v>48</v>
       </c>
       <c r="G29" s="3"/>
@@ -2146,7 +2158,7 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>134</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -2155,10 +2167,10 @@
       <c r="D30" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="F30" s="7" t="s">
         <v>182</v>
       </c>
       <c r="G30" s="3"/>
@@ -2168,19 +2180,19 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="14">
         <v>1.29</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="19" t="s">
         <v>78</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="7" t="s">
         <v>191</v>
       </c>
       <c r="G31" s="3"/>
@@ -2190,19 +2202,19 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="19" t="s">
         <v>78</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="7" t="s">
         <v>51</v>
       </c>
       <c r="G32" s="3"/>
@@ -2212,19 +2224,19 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="14">
         <v>1.31</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="19" t="s">
         <v>78</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E33" s="21" t="s">
+      <c r="E33" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="7" t="s">
         <v>172</v>
       </c>
       <c r="G33" s="3"/>
@@ -2234,15 +2246,15 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="15">
+      <c r="B34" s="14">
         <v>1.32</v>
       </c>
-      <c r="C34" s="20"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="21" t="s">
+      <c r="E34" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F34" s="12" t="s">
+      <c r="F34" s="7" t="s">
         <v>203</v>
       </c>
       <c r="G34" s="3"/>
@@ -2252,7 +2264,7 @@
         <f>+A34+1</f>
         <v>33</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="14" t="s">
         <v>131</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -2274,7 +2286,7 @@
         <f>+A35+1</f>
         <v>34</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="14" t="s">
         <v>132</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -2296,15 +2308,15 @@
         <f t="shared" ref="A37:A60" si="1">+A36+1</f>
         <v>35</v>
       </c>
-      <c r="B37" s="15">
+      <c r="B37" s="14">
         <v>1.35</v>
       </c>
-      <c r="C37" s="20"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="21" t="s">
+      <c r="E37" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="11" t="s">
         <v>188</v>
       </c>
       <c r="G37" s="3"/>
@@ -2314,15 +2326,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="14">
         <v>1.36</v>
       </c>
-      <c r="C38" s="20"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="21" t="s">
+      <c r="E38" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F38" s="11" t="s">
         <v>204</v>
       </c>
       <c r="G38" s="3"/>
@@ -2332,10 +2344,10 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="14">
         <v>1.37</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="19" t="s">
         <v>78</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -2344,7 +2356,7 @@
       <c r="E39" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="F39" s="11" t="s">
         <v>31</v>
       </c>
       <c r="G39" s="3"/>
@@ -2354,10 +2366,10 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B40" s="14">
         <v>1.38</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="19" t="s">
         <v>78</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -2366,7 +2378,7 @@
       <c r="E40" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F40" s="11" t="s">
         <v>59</v>
       </c>
       <c r="G40" s="3"/>
@@ -2376,19 +2388,19 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B41" s="14">
         <v>1.39</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="19" t="s">
         <v>78</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="11" t="s">
         <v>183</v>
       </c>
       <c r="G41" s="3"/>
@@ -2398,19 +2410,19 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="19" t="s">
         <v>282</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E42" s="21" t="s">
+      <c r="E42" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="F42" s="12" t="s">
+      <c r="F42" s="11" t="s">
         <v>175</v>
       </c>
       <c r="G42" s="3"/>
@@ -2420,7 +2432,7 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="14">
         <v>1.41</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2432,7 +2444,7 @@
       <c r="E43" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="F43" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G43" s="3"/>
@@ -2442,7 +2454,7 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="14">
         <v>1.42</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -2454,7 +2466,7 @@
       <c r="E44" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F44" s="11" t="s">
         <v>46</v>
       </c>
       <c r="G44" s="3"/>
@@ -2464,7 +2476,7 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B45" s="15">
+      <c r="B45" s="14">
         <v>1.43</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2476,101 +2488,101 @@
       <c r="E45" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="F45" s="11" t="s">
         <v>47</v>
       </c>
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="24">
+      <c r="A46" s="23">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B46" s="25">
+      <c r="B46" s="24">
         <v>1.44</v>
       </c>
-      <c r="C46" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46" s="24" t="s">
+      <c r="C46" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F46" s="11" t="s">
         <v>164</v>
       </c>
       <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="24">
+      <c r="A47" s="23">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B47" s="25">
+      <c r="B47" s="24">
         <v>1.45</v>
       </c>
-      <c r="C47" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="24" t="s">
+      <c r="C47" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="E47" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="F47" s="11" t="s">
         <v>209</v>
       </c>
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="24">
+      <c r="A48" s="23">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B48" s="25">
+      <c r="B48" s="24">
         <v>1.46</v>
       </c>
-      <c r="C48" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D48" s="24" t="s">
+      <c r="C48" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="E48" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" s="11" t="s">
         <v>200</v>
       </c>
       <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="24">
+      <c r="A49" s="23">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B49" s="25">
+      <c r="B49" s="24">
         <v>1.47</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="21" t="s">
+      <c r="E49" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F49" s="11" t="s">
         <v>207</v>
       </c>
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="24">
+      <c r="A50" s="23">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="14" t="s">
         <v>140</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -2582,17 +2594,17 @@
       <c r="E50" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="11" t="s">
         <v>61</v>
       </c>
       <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="24">
+      <c r="A51" s="23">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="14" t="s">
         <v>141</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -2604,17 +2616,17 @@
       <c r="E51" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F51" s="11" t="s">
         <v>58</v>
       </c>
       <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="24">
+      <c r="A52" s="23">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="14" t="s">
         <v>139</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -2626,17 +2638,17 @@
       <c r="E52" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="F52" s="13" t="s">
+      <c r="F52" s="12" t="s">
         <v>211</v>
       </c>
       <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="24">
+      <c r="A53" s="23">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="14" t="s">
         <v>283</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2648,17 +2660,17 @@
       <c r="E53" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="11" t="s">
         <v>54</v>
       </c>
       <c r="G53" s="3"/>
     </row>
     <row r="54" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="24">
+      <c r="A54" s="23">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="14" t="s">
         <v>284</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -2670,17 +2682,17 @@
       <c r="E54" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="F54" s="13" t="s">
+      <c r="F54" s="12" t="s">
         <v>195</v>
       </c>
       <c r="G54" s="3"/>
     </row>
     <row r="55" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="24">
+      <c r="A55" s="23">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="14" t="s">
         <v>285</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -2692,17 +2704,17 @@
       <c r="E55" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="F55" s="11" t="s">
         <v>56</v>
       </c>
       <c r="G55" s="3"/>
     </row>
     <row r="56" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="24">
+      <c r="A56" s="23">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="14" t="s">
         <v>286</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -2714,17 +2726,17 @@
       <c r="E56" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F56" s="11" t="s">
         <v>55</v>
       </c>
       <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="24">
+      <c r="A57" s="23">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="14">
         <v>1.55</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -2733,20 +2745,20 @@
       <c r="D57" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E57" s="21" t="s">
+      <c r="E57" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="F57" s="7" t="s">
         <v>166</v>
       </c>
       <c r="G57" s="3"/>
     </row>
     <row r="58" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="24">
+      <c r="A58" s="23">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="14" t="s">
         <v>288</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -2758,17 +2770,17 @@
       <c r="E58" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" s="11" t="s">
         <v>57</v>
       </c>
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="24">
+      <c r="A59" s="23">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="14" t="s">
         <v>287</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -2777,32 +2789,32 @@
       <c r="D59" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="E59" s="21" t="s">
+      <c r="E59" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="F59" s="12" t="s">
+      <c r="F59" s="11" t="s">
         <v>189</v>
       </c>
       <c r="G59" s="3"/>
     </row>
     <row r="60" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="24">
+      <c r="A60" s="23">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="B60" s="25" t="s">
+      <c r="B60" s="24" t="s">
         <v>290</v>
       </c>
-      <c r="C60" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D60" s="24" t="s">
+      <c r="C60" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D60" s="23" t="s">
         <v>289</v>
       </c>
-      <c r="E60" s="21" t="s">
+      <c r="E60" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F60" s="7" t="s">
         <v>202</v>
       </c>
       <c r="G60" s="3"/>
@@ -2812,139 +2824,139 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B61" s="25">
+      <c r="B61" s="24">
         <v>1.59</v>
       </c>
-      <c r="C61" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" s="24" t="s">
+      <c r="C61" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="E61" s="21" t="s">
+      <c r="E61" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F61" s="11" t="s">
         <v>205</v>
       </c>
       <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="24">
+      <c r="A62" s="23">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B62" s="25" t="s">
+      <c r="B62" s="24" t="s">
         <v>291</v>
       </c>
-      <c r="C62" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D62" s="24" t="s">
+      <c r="C62" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" s="23" t="s">
         <v>292</v>
       </c>
-      <c r="E62" s="21" t="s">
+      <c r="E62" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="F62" s="12" t="s">
+      <c r="F62" s="11" t="s">
         <v>179</v>
       </c>
       <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="24">
+      <c r="A63" s="23">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B63" s="25" t="s">
+      <c r="B63" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="C63" s="24" t="s">
+      <c r="C63" s="23" t="s">
         <v>78</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="E63" s="21" t="s">
+      <c r="E63" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="F63" s="12" t="s">
+      <c r="F63" s="11" t="s">
         <v>198</v>
       </c>
       <c r="G63" s="3"/>
     </row>
     <row r="64" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="24">
+      <c r="A64" s="23">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B64" s="25" t="s">
+      <c r="B64" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C64" s="23" t="s">
         <v>78</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="E64" s="21" t="s">
+      <c r="E64" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="F64" s="12" t="s">
+      <c r="F64" s="11" t="s">
         <v>197</v>
       </c>
       <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="24">
+      <c r="A65" s="23">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B65" s="25" t="s">
+      <c r="B65" s="24" t="s">
         <v>295</v>
       </c>
-      <c r="C65" s="24" t="s">
+      <c r="C65" s="23" t="s">
         <v>78</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="E65" s="21" t="s">
+      <c r="E65" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="F65" s="12" t="s">
+      <c r="F65" s="11" t="s">
         <v>181</v>
       </c>
       <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="24">
+      <c r="A66" s="23">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B66" s="15">
+      <c r="B66" s="14">
         <v>1.64</v>
       </c>
-      <c r="C66" s="24" t="s">
+      <c r="C66" s="23" t="s">
         <v>78</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="E66" s="21" t="s">
+      <c r="E66" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="F66" s="12" t="s">
+      <c r="F66" s="11" t="s">
         <v>194</v>
       </c>
       <c r="G66" s="3"/>
     </row>
     <row r="67" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="24">
+      <c r="A67" s="23">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B67" s="15">
+      <c r="B67" s="14">
         <v>1.65</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -2953,20 +2965,20 @@
       <c r="D67" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="E67" s="21" t="s">
+      <c r="E67" s="20" t="s">
         <v>312</v>
       </c>
-      <c r="F67" s="12" t="s">
+      <c r="F67" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G67" s="3"/>
     </row>
     <row r="68" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="24">
+      <c r="A68" s="23">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B68" s="15">
+      <c r="B68" s="14">
         <v>1.66</v>
       </c>
       <c r="C68" s="3" t="s">
@@ -2978,17 +2990,17 @@
       <c r="E68" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="F68" s="12" t="s">
+      <c r="F68" s="11" t="s">
         <v>45</v>
       </c>
       <c r="G68" s="3"/>
     </row>
     <row r="69" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="24">
+      <c r="A69" s="23">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="B69" s="15">
+      <c r="B69" s="14">
         <v>1.67</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -3000,17 +3012,17 @@
       <c r="E69" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="F69" s="12" t="s">
+      <c r="F69" s="11" t="s">
         <v>42</v>
       </c>
       <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="24">
+      <c r="A70" s="23">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="B70" s="15">
+      <c r="B70" s="14">
         <v>1.68</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -3022,17 +3034,17 @@
       <c r="E70" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F70" s="11" t="s">
         <v>43</v>
       </c>
       <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="24">
+      <c r="A71" s="23">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="B71" s="15">
+      <c r="B71" s="14">
         <v>1.69</v>
       </c>
       <c r="C71" s="3" t="s">
@@ -3044,17 +3056,17 @@
       <c r="E71" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F71" s="12" t="s">
+      <c r="F71" s="11" t="s">
         <v>44</v>
       </c>
       <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="24">
+      <c r="A72" s="23">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="B72" s="15" t="s">
+      <c r="B72" s="14" t="s">
         <v>301</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -3066,17 +3078,17 @@
       <c r="E72" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="F72" s="12" t="s">
+      <c r="F72" s="11" t="s">
         <v>71</v>
       </c>
       <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="24">
+      <c r="A73" s="23">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="B73" s="15">
+      <c r="B73" s="14">
         <v>1.71</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -3088,17 +3100,17 @@
       <c r="E73" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="F73" s="12" t="s">
+      <c r="F73" s="11" t="s">
         <v>72</v>
       </c>
       <c r="G73" s="3"/>
     </row>
     <row r="74" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="24">
+      <c r="A74" s="23">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="14" t="s">
         <v>302</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -3110,17 +3122,17 @@
       <c r="E74" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="F74" s="12" t="s">
+      <c r="F74" s="11" t="s">
         <v>6</v>
       </c>
       <c r="G74" s="3"/>
     </row>
     <row r="75" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="24">
+      <c r="A75" s="23">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-      <c r="B75" s="15" t="s">
+      <c r="B75" s="14" t="s">
         <v>303</v>
       </c>
       <c r="C75" s="3" t="s">
@@ -3129,20 +3141,20 @@
       <c r="D75" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E75" s="3" t="s">
+      <c r="E75" s="27" t="s">
         <v>251</v>
       </c>
-      <c r="F75" s="12" t="s">
+      <c r="F75" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G75" s="3"/>
     </row>
     <row r="76" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="24">
+      <c r="A76" s="23">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="B76" s="15">
+      <c r="B76" s="14">
         <v>1.74</v>
       </c>
       <c r="C76" s="3" t="s">
@@ -3154,17 +3166,17 @@
       <c r="E76" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="F76" s="12" t="s">
+      <c r="F76" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G76" s="3"/>
     </row>
     <row r="77" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="24">
+      <c r="A77" s="23">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="B77" s="15" t="s">
+      <c r="B77" s="14" t="s">
         <v>304</v>
       </c>
       <c r="C77" s="3" t="s">
@@ -3176,17 +3188,17 @@
       <c r="E77" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="F77" s="12" t="s">
+      <c r="F77" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G77" s="3"/>
     </row>
     <row r="78" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="24">
+      <c r="A78" s="23">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="B78" s="15" t="s">
+      <c r="B78" s="14" t="s">
         <v>305</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -3198,17 +3210,17 @@
       <c r="E78" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="F78" s="12" t="s">
+      <c r="F78" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G78" s="3"/>
     </row>
     <row r="79" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="24">
+      <c r="A79" s="23">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="B79" s="15" t="s">
+      <c r="B79" s="14" t="s">
         <v>306</v>
       </c>
       <c r="C79" s="3" t="s">
@@ -3220,17 +3232,17 @@
       <c r="E79" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="F79" s="12" t="s">
+      <c r="F79" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G79" s="3"/>
     </row>
     <row r="80" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="24">
-        <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-      <c r="B80" s="15" t="s">
+      <c r="A80" s="23">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="B80" s="14" t="s">
         <v>307</v>
       </c>
       <c r="C80" s="3" t="s">
@@ -3242,7 +3254,7 @@
       <c r="E80" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="F80" s="12" t="s">
+      <c r="F80" s="11" t="s">
         <v>14</v>
       </c>
       <c r="G80" s="3"/>
@@ -3252,7 +3264,7 @@
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="B81" s="15" t="s">
+      <c r="B81" s="14" t="s">
         <v>308</v>
       </c>
       <c r="C81" s="3" t="s">
@@ -3261,7 +3273,7 @@
       <c r="D81" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="E81" s="6" t="s">
         <v>257</v>
       </c>
       <c r="F81" s="7" t="s">
@@ -3274,7 +3286,7 @@
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="14" t="s">
         <v>309</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -3286,7 +3298,7 @@
       <c r="E82" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="F82" s="12" t="s">
+      <c r="F82" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G82" s="3"/>
@@ -3296,13 +3308,13 @@
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="B83" s="15" t="s">
+      <c r="B83" s="14" t="s">
         <v>311</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D83" s="23"/>
+      <c r="D83" s="22"/>
       <c r="E83" s="6" t="s">
         <v>186</v>
       </c>
@@ -3316,17 +3328,17 @@
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="B84" s="15" t="s">
+      <c r="B84" s="14" t="s">
         <v>310</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D84" s="23"/>
-      <c r="E84" s="21" t="s">
+      <c r="D84" s="22"/>
+      <c r="E84" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="F84" s="12" t="s">
+      <c r="F84" s="11" t="s">
         <v>213</v>
       </c>
       <c r="G84" s="3"/>
@@ -3336,7 +3348,7 @@
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
-      <c r="B85" s="15" t="s">
+      <c r="B85" s="14" t="s">
         <v>152</v>
       </c>
       <c r="C85" s="3" t="s">
@@ -3348,7 +3360,7 @@
       <c r="E85" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F85" s="12" t="s">
+      <c r="F85" s="11" t="s">
         <v>33</v>
       </c>
       <c r="G85" s="3"/>
@@ -3358,7 +3370,7 @@
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="B86" s="15" t="s">
+      <c r="B86" s="14" t="s">
         <v>110</v>
       </c>
       <c r="C86" s="3" t="s">
@@ -3370,7 +3382,7 @@
       <c r="E86" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F86" s="12" t="s">
+      <c r="F86" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G86" s="3"/>
@@ -3380,7 +3392,7 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="B87" s="15" t="s">
+      <c r="B87" s="14" t="s">
         <v>153</v>
       </c>
       <c r="C87" s="3" t="s">
@@ -3392,7 +3404,7 @@
       <c r="E87" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="F87" s="12" t="s">
+      <c r="F87" s="11" t="s">
         <v>4</v>
       </c>
       <c r="G87" s="3"/>
@@ -3402,7 +3414,7 @@
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
-      <c r="B88" s="15" t="s">
+      <c r="B88" s="14" t="s">
         <v>144</v>
       </c>
       <c r="C88" s="3" t="s">
@@ -3414,7 +3426,7 @@
       <c r="E88" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="F88" s="12" t="s">
+      <c r="F88" s="11" t="s">
         <v>277</v>
       </c>
       <c r="G88" s="3"/>
@@ -3424,7 +3436,7 @@
         <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="B89" s="15" t="s">
+      <c r="B89" s="14" t="s">
         <v>143</v>
       </c>
       <c r="C89" s="3" t="s">
@@ -3436,7 +3448,7 @@
       <c r="E89" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F89" s="12" t="s">
+      <c r="F89" s="11" t="s">
         <v>11</v>
       </c>
       <c r="G89" s="3"/>
@@ -3446,7 +3458,7 @@
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="B90" s="15" t="s">
+      <c r="B90" s="14" t="s">
         <v>106</v>
       </c>
       <c r="C90" s="3" t="s">
@@ -3458,7 +3470,7 @@
       <c r="E90" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F90" s="10" t="s">
+      <c r="F90" s="9" t="s">
         <v>278</v>
       </c>
       <c r="G90" s="3"/>
@@ -3468,7 +3480,7 @@
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="B91" s="15" t="s">
+      <c r="B91" s="14" t="s">
         <v>146</v>
       </c>
       <c r="C91" s="3" t="s">
@@ -3480,7 +3492,7 @@
       <c r="E91" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="F91" s="12" t="s">
+      <c r="F91" s="11" t="s">
         <v>18</v>
       </c>
       <c r="G91" s="3"/>
@@ -3490,7 +3502,7 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="B92" s="15" t="s">
+      <c r="B92" s="14" t="s">
         <v>147</v>
       </c>
       <c r="C92" s="3" t="s">
@@ -3502,7 +3514,7 @@
       <c r="E92" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="F92" s="12" t="s">
+      <c r="F92" s="11" t="s">
         <v>19</v>
       </c>
       <c r="G92" s="3"/>
@@ -3512,7 +3524,7 @@
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="14" t="s">
         <v>148</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -3524,7 +3536,7 @@
       <c r="E93" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="F93" s="12" t="s">
+      <c r="F93" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G93" s="3"/>
@@ -3534,7 +3546,7 @@
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-      <c r="B94" s="15" t="s">
+      <c r="B94" s="14" t="s">
         <v>145</v>
       </c>
       <c r="C94" s="3" t="s">
@@ -3546,7 +3558,7 @@
       <c r="E94" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="F94" s="12" t="s">
+      <c r="F94" s="11" t="s">
         <v>15</v>
       </c>
       <c r="G94" s="3"/>
@@ -3556,7 +3568,7 @@
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="B95" s="15" t="s">
+      <c r="B95" s="14" t="s">
         <v>107</v>
       </c>
       <c r="C95" s="3" t="s">
@@ -3568,7 +3580,7 @@
       <c r="E95" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="F95" s="12" t="s">
+      <c r="F95" s="11" t="s">
         <v>279</v>
       </c>
       <c r="G95" s="3"/>
@@ -3578,7 +3590,7 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-      <c r="B96" s="15" t="s">
+      <c r="B96" s="14" t="s">
         <v>114</v>
       </c>
       <c r="C96" s="3" t="s">
@@ -3590,7 +3602,7 @@
       <c r="E96" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="F96" s="12" t="s">
+      <c r="F96" s="11" t="s">
         <v>22</v>
       </c>
       <c r="G96" s="3"/>
@@ -3600,7 +3612,7 @@
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="B97" s="15" t="s">
+      <c r="B97" s="14" t="s">
         <v>108</v>
       </c>
       <c r="C97" s="3" t="s">
@@ -3612,7 +3624,7 @@
       <c r="E97" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="F97" s="12" t="s">
+      <c r="F97" s="11" t="s">
         <v>23</v>
       </c>
       <c r="G97" s="3"/>
@@ -3622,7 +3634,7 @@
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="B98" s="17" t="s">
+      <c r="B98" s="16" t="s">
         <v>109</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -3634,7 +3646,7 @@
       <c r="E98" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="F98" s="12" t="s">
+      <c r="F98" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G98" s="3"/>
@@ -3644,7 +3656,7 @@
         <f t="shared" si="0"/>
         <v>97</v>
       </c>
-      <c r="B99" s="15" t="s">
+      <c r="B99" s="14" t="s">
         <v>149</v>
       </c>
       <c r="C99" s="3" t="s">
@@ -3653,7 +3665,7 @@
       <c r="D99" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E99" s="9" t="s">
+      <c r="E99" s="26" t="s">
         <v>270</v>
       </c>
       <c r="F99" s="7" t="s">
@@ -3666,7 +3678,7 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="B100" s="15" t="s">
+      <c r="B100" s="14" t="s">
         <v>150</v>
       </c>
       <c r="C100" s="3" t="s">
@@ -3678,7 +3690,7 @@
       <c r="E100" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="F100" s="12" t="s">
+      <c r="F100" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G100" s="3"/>
@@ -3688,7 +3700,7 @@
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="B101" s="15" t="s">
+      <c r="B101" s="14" t="s">
         <v>151</v>
       </c>
       <c r="C101" s="3" t="s">
@@ -3700,7 +3712,7 @@
       <c r="E101" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="F101" s="12" t="s">
+      <c r="F101" s="11" t="s">
         <v>28</v>
       </c>
       <c r="G101" s="3"/>
@@ -3710,7 +3722,7 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="B102" s="15" t="s">
+      <c r="B102" s="14" t="s">
         <v>142</v>
       </c>
       <c r="C102" s="3" t="s">
@@ -3722,7 +3734,7 @@
       <c r="E102" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F102" s="12" t="s">
+      <c r="F102" s="11" t="s">
         <v>37</v>
       </c>
       <c r="G102" s="3"/>
@@ -3732,7 +3744,7 @@
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="B103" s="15" t="s">
+      <c r="B103" s="14" t="s">
         <v>111</v>
       </c>
       <c r="C103" s="3" t="s">
@@ -3744,7 +3756,7 @@
       <c r="E103" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F103" s="12" t="s">
+      <c r="F103" s="11" t="s">
         <v>38</v>
       </c>
       <c r="G103" s="3"/>
@@ -3754,7 +3766,7 @@
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="B104" s="15" t="s">
+      <c r="B104" s="14" t="s">
         <v>112</v>
       </c>
       <c r="C104" s="3" t="s">
@@ -3766,7 +3778,7 @@
       <c r="E104" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F104" s="12" t="s">
+      <c r="F104" s="11" t="s">
         <v>39</v>
       </c>
       <c r="G104" s="3"/>
@@ -3776,7 +3788,7 @@
         <f t="shared" si="0"/>
         <v>103</v>
       </c>
-      <c r="B105" s="15" t="s">
+      <c r="B105" s="14" t="s">
         <v>113</v>
       </c>
       <c r="C105" s="3" t="s">
@@ -3788,7 +3800,7 @@
       <c r="E105" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F105" s="12" t="s">
+      <c r="F105" s="11" t="s">
         <v>40</v>
       </c>
       <c r="G105" s="3"/>
@@ -3798,7 +3810,7 @@
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-      <c r="B106" s="15" t="s">
+      <c r="B106" s="14" t="s">
         <v>158</v>
       </c>
       <c r="C106" s="3" t="s">
@@ -3807,10 +3819,10 @@
       <c r="D106" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E106" s="21" t="s">
+      <c r="E106" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="F106" s="12" t="s">
+      <c r="F106" s="11" t="s">
         <v>280</v>
       </c>
       <c r="G106" s="3"/>
@@ -3820,7 +3832,7 @@
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="B107" s="15" t="s">
+      <c r="B107" s="14" t="s">
         <v>154</v>
       </c>
       <c r="C107" s="3" t="s">
@@ -3832,7 +3844,7 @@
       <c r="E107" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="F107" s="12" t="s">
+      <c r="F107" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G107" s="3"/>
@@ -3842,7 +3854,7 @@
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
-      <c r="B108" s="15" t="s">
+      <c r="B108" s="14" t="s">
         <v>155</v>
       </c>
       <c r="C108" s="3" t="s">
@@ -3854,7 +3866,7 @@
       <c r="E108" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="F108" s="12" t="s">
+      <c r="F108" s="11" t="s">
         <v>8</v>
       </c>
       <c r="G108" s="3"/>
@@ -3864,7 +3876,7 @@
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="B109" s="15" t="s">
+      <c r="B109" s="14" t="s">
         <v>156</v>
       </c>
       <c r="C109" s="3" t="s">
@@ -3876,7 +3888,7 @@
       <c r="E109" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="F109" s="12" t="s">
+      <c r="F109" s="11" t="s">
         <v>64</v>
       </c>
       <c r="G109" s="3"/>
@@ -3886,7 +3898,7 @@
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
-      <c r="B110" s="15" t="s">
+      <c r="B110" s="14" t="s">
         <v>157</v>
       </c>
       <c r="C110" s="3" t="s">
@@ -3898,86 +3910,86 @@
       <c r="E110" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="F110" s="12" t="s">
+      <c r="F110" s="11" t="s">
         <v>36</v>
       </c>
       <c r="G110" s="3"/>
     </row>
     <row r="111" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
-      <c r="B111" s="22"/>
-      <c r="C111" s="23"/>
-      <c r="D111" s="23"/>
-      <c r="E111" s="23"/>
-      <c r="F111" s="23"/>
+      <c r="B111" s="21"/>
+      <c r="C111" s="22"/>
+      <c r="D111" s="22"/>
+      <c r="E111" s="22"/>
+      <c r="F111" s="22"/>
       <c r="G111" s="3"/>
     </row>
     <row r="112" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
-      <c r="B112" s="22"/>
-      <c r="C112" s="23"/>
-      <c r="D112" s="23"/>
-      <c r="E112" s="23"/>
-      <c r="F112" s="23"/>
+      <c r="B112" s="21"/>
+      <c r="C112" s="22"/>
+      <c r="D112" s="22"/>
+      <c r="E112" s="22"/>
+      <c r="F112" s="22"/>
       <c r="G112" s="3"/>
     </row>
     <row r="113" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
-      <c r="B113" s="22"/>
-      <c r="C113" s="23"/>
-      <c r="D113" s="23"/>
-      <c r="E113" s="23"/>
-      <c r="F113" s="23"/>
+      <c r="B113" s="21"/>
+      <c r="C113" s="22"/>
+      <c r="D113" s="22"/>
+      <c r="E113" s="22"/>
+      <c r="F113" s="22"/>
       <c r="G113" s="3"/>
     </row>
     <row r="114" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
-      <c r="B114" s="22"/>
-      <c r="C114" s="23"/>
-      <c r="D114" s="23"/>
-      <c r="E114" s="23"/>
-      <c r="F114" s="23"/>
+      <c r="B114" s="21"/>
+      <c r="C114" s="22"/>
+      <c r="D114" s="22"/>
+      <c r="E114" s="22"/>
+      <c r="F114" s="22"/>
       <c r="G114" s="3"/>
     </row>
     <row r="115" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
-      <c r="B115" s="22"/>
-      <c r="C115" s="23"/>
-      <c r="D115" s="23"/>
-      <c r="E115" s="23"/>
-      <c r="F115" s="23"/>
+      <c r="B115" s="21"/>
+      <c r="C115" s="22"/>
+      <c r="D115" s="22"/>
+      <c r="E115" s="22"/>
+      <c r="F115" s="22"/>
       <c r="G115" s="3"/>
     </row>
     <row r="116" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
-      <c r="B116" s="22"/>
-      <c r="C116" s="23"/>
-      <c r="D116" s="23"/>
-      <c r="E116" s="23"/>
-      <c r="F116" s="23"/>
+      <c r="B116" s="21"/>
+      <c r="C116" s="22"/>
+      <c r="D116" s="22"/>
+      <c r="E116" s="22"/>
+      <c r="F116" s="22"/>
       <c r="G116" s="3"/>
     </row>
     <row r="117" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
-      <c r="B117" s="22"/>
-      <c r="C117" s="23"/>
-      <c r="D117" s="23"/>
-      <c r="E117" s="23"/>
-      <c r="F117" s="23"/>
+      <c r="B117" s="21"/>
+      <c r="C117" s="22"/>
+      <c r="D117" s="22"/>
+      <c r="E117" s="22"/>
+      <c r="F117" s="22"/>
       <c r="G117" s="3"/>
     </row>
     <row r="118" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
-      <c r="B118" s="22"/>
-      <c r="C118" s="23"/>
-      <c r="D118" s="23"/>
-      <c r="E118" s="23"/>
-      <c r="F118" s="23"/>
+      <c r="B118" s="21"/>
+      <c r="C118" s="22"/>
+      <c r="D118" s="22"/>
+      <c r="E118" s="22"/>
+      <c r="F118" s="22"/>
       <c r="G118" s="3"/>
     </row>
     <row r="119" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
-      <c r="B119" s="18"/>
+      <c r="B119" s="17"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
@@ -3989,11 +4001,11 @@
     <row r="126" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="D126" s="8"/>
       <c r="E126" s="8"/>
-      <c r="F126" s="11"/>
+      <c r="F126" s="10"/>
     </row>
     <row r="129" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
       <c r="E129" s="8"/>
-      <c r="F129" s="11"/>
+      <c r="F129" s="10"/>
     </row>
     <row r="133" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="D133" s="8"/>

</xml_diff>

<commit_message>
Ghana Mala edit TS 1.4,1.6 Ghanam edited - 28/07/2022
</commit_message>
<xml_diff>
--- a/Ghana Maala/Ghana Maala Content.xlsx
+++ b/Ghana Maala/Ghana Maala Content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\Ghana Maala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB34DF3-E892-47B2-8E32-248388CE0CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CD1574-9A97-43E8-990E-A5A59159863E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="313">
   <si>
     <t>Ghanam Description</t>
   </si>
@@ -980,7 +980,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1007,8 +1007,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1018,12 +1023,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1107,7 +1106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1129,16 +1128,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1182,6 +1178,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1524,14 +1526,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="17" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
@@ -1541,7 +1543,7 @@
   <sheetData>
     <row r="2" spans="1:7" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>105</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1564,7 +1566,7 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>115</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1586,7 +1588,7 @@
         <f>+A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>116</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1608,7 +1610,7 @@
         <f t="shared" ref="A5:A110" si="0">+A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>117</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1630,7 +1632,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <v>1.4</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1652,7 +1654,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>1.5</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1674,7 +1676,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>1.6</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1696,7 +1698,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>1.7</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1718,7 +1720,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <v>1.8</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1740,7 +1742,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>1.9</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1762,7 +1764,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>118</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1784,7 +1786,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>119</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1793,10 +1795,10 @@
       <c r="D13" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="12" t="s">
         <v>171</v>
       </c>
       <c r="G13" s="3"/>
@@ -1806,7 +1808,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>120</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1828,7 +1830,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>121</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1850,7 +1852,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>281</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1872,7 +1874,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>122</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1894,7 +1896,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="13">
         <v>1.1599999999999999</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1903,10 +1905,10 @@
       <c r="D18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="12" t="s">
         <v>169</v>
       </c>
       <c r="G18" s="3"/>
@@ -1916,7 +1918,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>125</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1938,7 +1940,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>124</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1950,7 +1952,7 @@
       <c r="E20" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>177</v>
       </c>
       <c r="G20" s="3"/>
@@ -1960,7 +1962,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>123</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1972,7 +1974,7 @@
       <c r="E21" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="10" t="s">
         <v>62</v>
       </c>
       <c r="G21" s="3"/>
@@ -1982,7 +1984,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>127</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1994,7 +1996,7 @@
       <c r="E22" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>63</v>
       </c>
       <c r="G22" s="3"/>
@@ -2004,7 +2006,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>128</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -2016,7 +2018,7 @@
       <c r="E23" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="10" t="s">
         <v>24</v>
       </c>
       <c r="G23" s="3"/>
@@ -2026,7 +2028,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>135</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -2038,7 +2040,7 @@
       <c r="E24" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>60</v>
       </c>
       <c r="G24" s="3"/>
@@ -2048,7 +2050,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>126</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -2060,7 +2062,7 @@
       <c r="E25" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="10" t="s">
         <v>30</v>
       </c>
       <c r="G25" s="3"/>
@@ -2070,7 +2072,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>138</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -2092,7 +2094,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>129</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2101,10 +2103,10 @@
       <c r="D27" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="7" t="s">
         <v>49</v>
       </c>
       <c r="G27" s="3"/>
@@ -2114,7 +2116,7 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>130</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2126,7 +2128,7 @@
       <c r="E28" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="10" t="s">
         <v>50</v>
       </c>
       <c r="G28" s="3"/>
@@ -2136,7 +2138,7 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>133</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -2148,7 +2150,7 @@
       <c r="E29" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="10" t="s">
         <v>48</v>
       </c>
       <c r="G29" s="3"/>
@@ -2158,7 +2160,7 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>134</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -2167,7 +2169,7 @@
       <c r="D30" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="26" t="s">
         <v>184</v>
       </c>
       <c r="F30" s="7" t="s">
@@ -2180,10 +2182,10 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="13">
         <v>1.29</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="18" t="s">
         <v>78</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -2202,10 +2204,10 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="18" t="s">
         <v>78</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -2224,10 +2226,10 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="13">
         <v>1.31</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="18" t="s">
         <v>78</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -2246,10 +2248,10 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="13">
         <v>1.32</v>
       </c>
-      <c r="C34" s="19"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="3"/>
       <c r="E34" s="6" t="s">
         <v>162</v>
@@ -2264,7 +2266,7 @@
         <f>+A34+1</f>
         <v>33</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="13" t="s">
         <v>131</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -2286,7 +2288,7 @@
         <f>+A35+1</f>
         <v>34</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="13" t="s">
         <v>132</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -2308,15 +2310,15 @@
         <f t="shared" ref="A37:A60" si="1">+A36+1</f>
         <v>35</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B37" s="13">
         <v>1.35</v>
       </c>
-      <c r="C37" s="19"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="20" t="s">
+      <c r="E37" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="10" t="s">
         <v>188</v>
       </c>
       <c r="G37" s="3"/>
@@ -2326,15 +2328,15 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="13">
         <v>1.36</v>
       </c>
-      <c r="C38" s="19"/>
+      <c r="C38" s="18"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="20" t="s">
+      <c r="E38" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="10" t="s">
         <v>204</v>
       </c>
       <c r="G38" s="3"/>
@@ -2344,10 +2346,10 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B39" s="14">
+      <c r="B39" s="13">
         <v>1.37</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="18" t="s">
         <v>78</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -2356,7 +2358,7 @@
       <c r="E39" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="10" t="s">
         <v>31</v>
       </c>
       <c r="G39" s="3"/>
@@ -2366,10 +2368,10 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B40" s="14">
+      <c r="B40" s="13">
         <v>1.38</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="18" t="s">
         <v>78</v>
       </c>
       <c r="D40" s="3" t="s">
@@ -2378,7 +2380,7 @@
       <c r="E40" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F40" s="10" t="s">
         <v>59</v>
       </c>
       <c r="G40" s="3"/>
@@ -2388,19 +2390,19 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B41" s="14">
+      <c r="B41" s="13">
         <v>1.39</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="18" t="s">
         <v>78</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="10" t="s">
         <v>183</v>
       </c>
       <c r="G41" s="3"/>
@@ -2410,19 +2412,19 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="18" t="s">
         <v>282</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="E42" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="28" t="s">
         <v>175</v>
       </c>
       <c r="G42" s="3"/>
@@ -2432,7 +2434,7 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B43" s="14">
+      <c r="B43" s="13">
         <v>1.41</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2441,10 +2443,10 @@
       <c r="D43" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G43" s="3"/>
@@ -2454,7 +2456,7 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B44" s="14">
+      <c r="B44" s="13">
         <v>1.42</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -2466,7 +2468,7 @@
       <c r="E44" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="F44" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G44" s="3"/>
@@ -2476,7 +2478,7 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B45" s="14">
+      <c r="B45" s="13">
         <v>1.43</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2485,104 +2487,108 @@
       <c r="D45" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="7" t="s">
         <v>47</v>
       </c>
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="23">
+      <c r="A46" s="22">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B46" s="24">
+      <c r="B46" s="23">
         <v>1.44</v>
       </c>
-      <c r="C46" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46" s="23" t="s">
+      <c r="C46" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E46" s="20" t="s">
+      <c r="E46" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="F46" s="7" t="s">
         <v>164</v>
       </c>
       <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="23">
+      <c r="A47" s="22">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B47" s="24">
+      <c r="B47" s="23">
         <v>1.45</v>
       </c>
-      <c r="C47" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="23" t="s">
+      <c r="C47" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E47" s="20" t="s">
+      <c r="E47" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="F47" s="10" t="s">
         <v>209</v>
       </c>
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="23">
+      <c r="A48" s="22">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B48" s="24">
+      <c r="B48" s="23">
         <v>1.46</v>
       </c>
-      <c r="C48" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D48" s="23" t="s">
+      <c r="C48" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E48" s="20" t="s">
+      <c r="E48" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="F48" s="11" t="s">
+      <c r="F48" s="7" t="s">
         <v>200</v>
       </c>
       <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23">
+      <c r="A49" s="22">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B49" s="24">
+      <c r="B49" s="23">
         <v>1.47</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="20" t="s">
+      <c r="C49" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F49" s="7" t="s">
         <v>207</v>
       </c>
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="23">
+      <c r="A50" s="22">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="13" t="s">
         <v>140</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -2594,17 +2600,17 @@
       <c r="E50" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="F50" s="11" t="s">
+      <c r="F50" s="10" t="s">
         <v>61</v>
       </c>
       <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="23">
+      <c r="A51" s="22">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="13" t="s">
         <v>141</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -2616,17 +2622,17 @@
       <c r="E51" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F51" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="23">
+      <c r="A52" s="22">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="13" t="s">
         <v>139</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -2638,17 +2644,17 @@
       <c r="E52" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="11" t="s">
         <v>211</v>
       </c>
       <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="23">
+      <c r="A53" s="22">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="13" t="s">
         <v>283</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2660,17 +2666,17 @@
       <c r="E53" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="F53" s="10" t="s">
         <v>54</v>
       </c>
       <c r="G53" s="3"/>
     </row>
     <row r="54" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="23">
+      <c r="A54" s="22">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="13" t="s">
         <v>284</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -2682,17 +2688,17 @@
       <c r="E54" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="11" t="s">
         <v>195</v>
       </c>
       <c r="G54" s="3"/>
     </row>
     <row r="55" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="23">
+      <c r="A55" s="22">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="13" t="s">
         <v>285</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -2704,17 +2710,17 @@
       <c r="E55" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="F55" s="10" t="s">
         <v>56</v>
       </c>
       <c r="G55" s="3"/>
     </row>
     <row r="56" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="23">
+      <c r="A56" s="22">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="13" t="s">
         <v>286</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -2726,17 +2732,17 @@
       <c r="E56" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="F56" s="11" t="s">
+      <c r="F56" s="10" t="s">
         <v>55</v>
       </c>
       <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="23">
+      <c r="A57" s="22">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="B57" s="14">
+      <c r="B57" s="13">
         <v>1.55</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -2754,11 +2760,11 @@
       <c r="G57" s="3"/>
     </row>
     <row r="58" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="23">
+      <c r="A58" s="22">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="13" t="s">
         <v>288</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -2770,17 +2776,17 @@
       <c r="E58" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="F58" s="11" t="s">
+      <c r="F58" s="10" t="s">
         <v>57</v>
       </c>
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="23">
+      <c r="A59" s="22">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="13" t="s">
         <v>287</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -2789,26 +2795,26 @@
       <c r="D59" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="E59" s="20" t="s">
+      <c r="E59" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F59" s="10" t="s">
         <v>189</v>
       </c>
       <c r="G59" s="3"/>
     </row>
     <row r="60" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="23">
+      <c r="A60" s="22">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="B60" s="24" t="s">
+      <c r="B60" s="23" t="s">
         <v>290</v>
       </c>
-      <c r="C60" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D60" s="23" t="s">
+      <c r="C60" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D60" s="22" t="s">
         <v>289</v>
       </c>
       <c r="E60" s="6" t="s">
@@ -2824,139 +2830,139 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B61" s="24">
+      <c r="B61" s="23">
         <v>1.59</v>
       </c>
-      <c r="C61" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" s="23" t="s">
+      <c r="C61" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="E61" s="20" t="s">
+      <c r="E61" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="F61" s="11" t="s">
+      <c r="F61" s="10" t="s">
         <v>205</v>
       </c>
       <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="23">
+      <c r="A62" s="22">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B62" s="24" t="s">
+      <c r="B62" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="C62" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="D62" s="23" t="s">
+      <c r="C62" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="E62" s="20" t="s">
+      <c r="E62" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="F62" s="11" t="s">
+      <c r="F62" s="10" t="s">
         <v>179</v>
       </c>
       <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="23">
+      <c r="A63" s="22">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B63" s="24" t="s">
+      <c r="B63" s="23" t="s">
         <v>293</v>
       </c>
-      <c r="C63" s="23" t="s">
+      <c r="C63" s="22" t="s">
         <v>78</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="E63" s="20" t="s">
+      <c r="E63" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="F63" s="11" t="s">
+      <c r="F63" s="10" t="s">
         <v>198</v>
       </c>
       <c r="G63" s="3"/>
     </row>
     <row r="64" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="23">
+      <c r="A64" s="22">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B64" s="24" t="s">
+      <c r="B64" s="23" t="s">
         <v>294</v>
       </c>
-      <c r="C64" s="23" t="s">
+      <c r="C64" s="22" t="s">
         <v>78</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="E64" s="20" t="s">
+      <c r="E64" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="F64" s="11" t="s">
+      <c r="F64" s="10" t="s">
         <v>197</v>
       </c>
       <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="23">
+      <c r="A65" s="22">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B65" s="24" t="s">
+      <c r="B65" s="23" t="s">
         <v>295</v>
       </c>
-      <c r="C65" s="23" t="s">
+      <c r="C65" s="22" t="s">
         <v>78</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="E65" s="20" t="s">
+      <c r="E65" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="F65" s="11" t="s">
+      <c r="F65" s="10" t="s">
         <v>181</v>
       </c>
       <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="23">
+      <c r="A66" s="22">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B66" s="14">
+      <c r="B66" s="13">
         <v>1.64</v>
       </c>
-      <c r="C66" s="23" t="s">
+      <c r="C66" s="22" t="s">
         <v>78</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="E66" s="20" t="s">
+      <c r="E66" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="F66" s="11" t="s">
+      <c r="F66" s="10" t="s">
         <v>194</v>
       </c>
       <c r="G66" s="3"/>
     </row>
     <row r="67" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="23">
+      <c r="A67" s="22">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B67" s="14">
+      <c r="B67" s="13">
         <v>1.65</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -2965,20 +2971,20 @@
       <c r="D67" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="E67" s="20" t="s">
+      <c r="E67" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="F67" s="11" t="s">
+      <c r="F67" s="10" t="s">
         <v>17</v>
       </c>
       <c r="G67" s="3"/>
     </row>
     <row r="68" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="23">
+      <c r="A68" s="22">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B68" s="14">
+      <c r="B68" s="13">
         <v>1.66</v>
       </c>
       <c r="C68" s="3" t="s">
@@ -2990,17 +2996,17 @@
       <c r="E68" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="F68" s="11" t="s">
+      <c r="F68" s="10" t="s">
         <v>45</v>
       </c>
       <c r="G68" s="3"/>
     </row>
     <row r="69" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="23">
+      <c r="A69" s="22">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="B69" s="14">
+      <c r="B69" s="13">
         <v>1.67</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -3012,17 +3018,17 @@
       <c r="E69" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="F69" s="11" t="s">
+      <c r="F69" s="10" t="s">
         <v>42</v>
       </c>
       <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="23">
+      <c r="A70" s="22">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="B70" s="14">
+      <c r="B70" s="13">
         <v>1.68</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -3034,17 +3040,17 @@
       <c r="E70" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="F70" s="11" t="s">
+      <c r="F70" s="10" t="s">
         <v>43</v>
       </c>
       <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="23">
+      <c r="A71" s="22">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="B71" s="14">
+      <c r="B71" s="13">
         <v>1.69</v>
       </c>
       <c r="C71" s="3" t="s">
@@ -3056,17 +3062,17 @@
       <c r="E71" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="F71" s="11" t="s">
+      <c r="F71" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="23">
+      <c r="A72" s="22">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="13" t="s">
         <v>301</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -3078,17 +3084,17 @@
       <c r="E72" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="F72" s="11" t="s">
+      <c r="F72" s="10" t="s">
         <v>71</v>
       </c>
       <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="23">
+      <c r="A73" s="22">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="B73" s="14">
+      <c r="B73" s="13">
         <v>1.71</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -3100,17 +3106,17 @@
       <c r="E73" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="F73" s="11" t="s">
+      <c r="F73" s="10" t="s">
         <v>72</v>
       </c>
       <c r="G73" s="3"/>
     </row>
     <row r="74" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="23">
+      <c r="A74" s="22">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="13" t="s">
         <v>302</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -3122,17 +3128,17 @@
       <c r="E74" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="F74" s="11" t="s">
+      <c r="F74" s="10" t="s">
         <v>6</v>
       </c>
       <c r="G74" s="3"/>
     </row>
     <row r="75" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="23">
+      <c r="A75" s="22">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B75" s="13" t="s">
         <v>303</v>
       </c>
       <c r="C75" s="3" t="s">
@@ -3141,7 +3147,7 @@
       <c r="D75" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E75" s="27" t="s">
+      <c r="E75" s="26" t="s">
         <v>251</v>
       </c>
       <c r="F75" s="7" t="s">
@@ -3150,11 +3156,11 @@
       <c r="G75" s="3"/>
     </row>
     <row r="76" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="23">
+      <c r="A76" s="22">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="B76" s="14">
+      <c r="B76" s="13">
         <v>1.74</v>
       </c>
       <c r="C76" s="3" t="s">
@@ -3166,17 +3172,17 @@
       <c r="E76" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="F76" s="11" t="s">
+      <c r="F76" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G76" s="3"/>
     </row>
     <row r="77" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="23">
+      <c r="A77" s="22">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="13" t="s">
         <v>304</v>
       </c>
       <c r="C77" s="3" t="s">
@@ -3188,17 +3194,17 @@
       <c r="E77" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="F77" s="11" t="s">
+      <c r="F77" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G77" s="3"/>
     </row>
     <row r="78" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="23">
+      <c r="A78" s="22">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="13" t="s">
         <v>305</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -3210,17 +3216,17 @@
       <c r="E78" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="F78" s="11" t="s">
+      <c r="F78" s="10" t="s">
         <v>32</v>
       </c>
       <c r="G78" s="3"/>
     </row>
     <row r="79" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="23">
+      <c r="A79" s="22">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="13" t="s">
         <v>306</v>
       </c>
       <c r="C79" s="3" t="s">
@@ -3232,17 +3238,17 @@
       <c r="E79" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="F79" s="11" t="s">
+      <c r="F79" s="10" t="s">
         <v>16</v>
       </c>
       <c r="G79" s="3"/>
     </row>
     <row r="80" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="23">
-        <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-      <c r="B80" s="14" t="s">
+      <c r="A80" s="22">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="B80" s="13" t="s">
         <v>307</v>
       </c>
       <c r="C80" s="3" t="s">
@@ -3254,7 +3260,7 @@
       <c r="E80" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="F80" s="11" t="s">
+      <c r="F80" s="10" t="s">
         <v>14</v>
       </c>
       <c r="G80" s="3"/>
@@ -3264,7 +3270,7 @@
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="B81" s="14" t="s">
+      <c r="B81" s="13" t="s">
         <v>308</v>
       </c>
       <c r="C81" s="3" t="s">
@@ -3286,7 +3292,7 @@
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="B82" s="14" t="s">
+      <c r="B82" s="13" t="s">
         <v>309</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -3298,7 +3304,7 @@
       <c r="E82" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="F82" s="11" t="s">
+      <c r="F82" s="10" t="s">
         <v>29</v>
       </c>
       <c r="G82" s="3"/>
@@ -3308,13 +3314,13 @@
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="B83" s="14" t="s">
+      <c r="B83" s="13" t="s">
         <v>311</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D83" s="22"/>
+      <c r="D83" s="21"/>
       <c r="E83" s="6" t="s">
         <v>186</v>
       </c>
@@ -3328,17 +3334,17 @@
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B84" s="13" t="s">
         <v>310</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D84" s="22"/>
-      <c r="E84" s="20" t="s">
+      <c r="D84" s="21"/>
+      <c r="E84" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="F84" s="11" t="s">
+      <c r="F84" s="10" t="s">
         <v>213</v>
       </c>
       <c r="G84" s="3"/>
@@ -3348,7 +3354,7 @@
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B85" s="13" t="s">
         <v>152</v>
       </c>
       <c r="C85" s="3" t="s">
@@ -3360,7 +3366,7 @@
       <c r="E85" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F85" s="11" t="s">
+      <c r="F85" s="10" t="s">
         <v>33</v>
       </c>
       <c r="G85" s="3"/>
@@ -3370,7 +3376,7 @@
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="13" t="s">
         <v>110</v>
       </c>
       <c r="C86" s="3" t="s">
@@ -3382,7 +3388,7 @@
       <c r="E86" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F86" s="11" t="s">
+      <c r="F86" s="10" t="s">
         <v>3</v>
       </c>
       <c r="G86" s="3"/>
@@ -3392,7 +3398,7 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B87" s="13" t="s">
         <v>153</v>
       </c>
       <c r="C87" s="3" t="s">
@@ -3404,7 +3410,7 @@
       <c r="E87" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="F87" s="11" t="s">
+      <c r="F87" s="10" t="s">
         <v>4</v>
       </c>
       <c r="G87" s="3"/>
@@ -3414,7 +3420,7 @@
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
-      <c r="B88" s="14" t="s">
+      <c r="B88" s="13" t="s">
         <v>144</v>
       </c>
       <c r="C88" s="3" t="s">
@@ -3426,7 +3432,7 @@
       <c r="E88" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="F88" s="11" t="s">
+      <c r="F88" s="10" t="s">
         <v>277</v>
       </c>
       <c r="G88" s="3"/>
@@ -3436,7 +3442,7 @@
         <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="B89" s="14" t="s">
+      <c r="B89" s="13" t="s">
         <v>143</v>
       </c>
       <c r="C89" s="3" t="s">
@@ -3445,10 +3451,10 @@
       <c r="D89" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E89" s="3" t="s">
+      <c r="E89" s="26" t="s">
         <v>262</v>
       </c>
-      <c r="F89" s="11" t="s">
+      <c r="F89" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G89" s="3"/>
@@ -3458,7 +3464,7 @@
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B90" s="13" t="s">
         <v>106</v>
       </c>
       <c r="C90" s="3" t="s">
@@ -3467,10 +3473,10 @@
       <c r="D90" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E90" s="3" t="s">
+      <c r="E90" s="26" t="s">
         <v>262</v>
       </c>
-      <c r="F90" s="9" t="s">
+      <c r="F90" s="7" t="s">
         <v>278</v>
       </c>
       <c r="G90" s="3"/>
@@ -3480,7 +3486,7 @@
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B91" s="13" t="s">
         <v>146</v>
       </c>
       <c r="C91" s="3" t="s">
@@ -3492,7 +3498,7 @@
       <c r="E91" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="F91" s="11" t="s">
+      <c r="F91" s="10" t="s">
         <v>18</v>
       </c>
       <c r="G91" s="3"/>
@@ -3502,7 +3508,7 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B92" s="13" t="s">
         <v>147</v>
       </c>
       <c r="C92" s="3" t="s">
@@ -3514,7 +3520,7 @@
       <c r="E92" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="F92" s="11" t="s">
+      <c r="F92" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G92" s="3"/>
@@ -3524,7 +3530,7 @@
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B93" s="13" t="s">
         <v>148</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -3536,7 +3542,7 @@
       <c r="E93" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="F93" s="11" t="s">
+      <c r="F93" s="10" t="s">
         <v>20</v>
       </c>
       <c r="G93" s="3"/>
@@ -3546,7 +3552,7 @@
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="B94" s="13" t="s">
         <v>145</v>
       </c>
       <c r="C94" s="3" t="s">
@@ -3558,7 +3564,7 @@
       <c r="E94" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="F94" s="11" t="s">
+      <c r="F94" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G94" s="3"/>
@@ -3568,7 +3574,7 @@
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B95" s="13" t="s">
         <v>107</v>
       </c>
       <c r="C95" s="3" t="s">
@@ -3580,7 +3586,7 @@
       <c r="E95" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="F95" s="11" t="s">
+      <c r="F95" s="10" t="s">
         <v>279</v>
       </c>
       <c r="G95" s="3"/>
@@ -3590,7 +3596,7 @@
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-      <c r="B96" s="14" t="s">
+      <c r="B96" s="13" t="s">
         <v>114</v>
       </c>
       <c r="C96" s="3" t="s">
@@ -3602,7 +3608,7 @@
       <c r="E96" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="F96" s="11" t="s">
+      <c r="F96" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G96" s="3"/>
@@ -3612,7 +3618,7 @@
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="B97" s="14" t="s">
+      <c r="B97" s="13" t="s">
         <v>108</v>
       </c>
       <c r="C97" s="3" t="s">
@@ -3624,7 +3630,7 @@
       <c r="E97" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="F97" s="11" t="s">
+      <c r="F97" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G97" s="3"/>
@@ -3634,7 +3640,7 @@
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="B98" s="16" t="s">
+      <c r="B98" s="15" t="s">
         <v>109</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -3646,7 +3652,7 @@
       <c r="E98" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="F98" s="11" t="s">
+      <c r="F98" s="10" t="s">
         <v>21</v>
       </c>
       <c r="G98" s="3"/>
@@ -3656,7 +3662,7 @@
         <f t="shared" si="0"/>
         <v>97</v>
       </c>
-      <c r="B99" s="14" t="s">
+      <c r="B99" s="13" t="s">
         <v>149</v>
       </c>
       <c r="C99" s="3" t="s">
@@ -3665,7 +3671,7 @@
       <c r="D99" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E99" s="26" t="s">
+      <c r="E99" s="25" t="s">
         <v>270</v>
       </c>
       <c r="F99" s="7" t="s">
@@ -3678,7 +3684,7 @@
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="B100" s="14" t="s">
+      <c r="B100" s="13" t="s">
         <v>150</v>
       </c>
       <c r="C100" s="3" t="s">
@@ -3690,7 +3696,7 @@
       <c r="E100" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="F100" s="11" t="s">
+      <c r="F100" s="10" t="s">
         <v>25</v>
       </c>
       <c r="G100" s="3"/>
@@ -3700,7 +3706,7 @@
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="B101" s="14" t="s">
+      <c r="B101" s="13" t="s">
         <v>151</v>
       </c>
       <c r="C101" s="3" t="s">
@@ -3712,7 +3718,7 @@
       <c r="E101" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="F101" s="11" t="s">
+      <c r="F101" s="10" t="s">
         <v>28</v>
       </c>
       <c r="G101" s="3"/>
@@ -3722,7 +3728,7 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="B102" s="14" t="s">
+      <c r="B102" s="13" t="s">
         <v>142</v>
       </c>
       <c r="C102" s="3" t="s">
@@ -3734,7 +3740,7 @@
       <c r="E102" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F102" s="11" t="s">
+      <c r="F102" s="10" t="s">
         <v>37</v>
       </c>
       <c r="G102" s="3"/>
@@ -3744,7 +3750,7 @@
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="B103" s="13" t="s">
         <v>111</v>
       </c>
       <c r="C103" s="3" t="s">
@@ -3756,7 +3762,7 @@
       <c r="E103" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F103" s="11" t="s">
+      <c r="F103" s="10" t="s">
         <v>38</v>
       </c>
       <c r="G103" s="3"/>
@@ -3766,7 +3772,7 @@
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="B104" s="14" t="s">
+      <c r="B104" s="13" t="s">
         <v>112</v>
       </c>
       <c r="C104" s="3" t="s">
@@ -3778,7 +3784,7 @@
       <c r="E104" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F104" s="11" t="s">
+      <c r="F104" s="10" t="s">
         <v>39</v>
       </c>
       <c r="G104" s="3"/>
@@ -3788,7 +3794,7 @@
         <f t="shared" si="0"/>
         <v>103</v>
       </c>
-      <c r="B105" s="14" t="s">
+      <c r="B105" s="13" t="s">
         <v>113</v>
       </c>
       <c r="C105" s="3" t="s">
@@ -3800,7 +3806,7 @@
       <c r="E105" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F105" s="11" t="s">
+      <c r="F105" s="10" t="s">
         <v>40</v>
       </c>
       <c r="G105" s="3"/>
@@ -3810,7 +3816,7 @@
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-      <c r="B106" s="14" t="s">
+      <c r="B106" s="13" t="s">
         <v>158</v>
       </c>
       <c r="C106" s="3" t="s">
@@ -3819,10 +3825,10 @@
       <c r="D106" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E106" s="20" t="s">
+      <c r="E106" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="F106" s="11" t="s">
+      <c r="F106" s="10" t="s">
         <v>280</v>
       </c>
       <c r="G106" s="3"/>
@@ -3832,7 +3838,7 @@
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="B107" s="14" t="s">
+      <c r="B107" s="13" t="s">
         <v>154</v>
       </c>
       <c r="C107" s="3" t="s">
@@ -3844,7 +3850,7 @@
       <c r="E107" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="F107" s="11" t="s">
+      <c r="F107" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G107" s="3"/>
@@ -3854,7 +3860,7 @@
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
-      <c r="B108" s="14" t="s">
+      <c r="B108" s="13" t="s">
         <v>155</v>
       </c>
       <c r="C108" s="3" t="s">
@@ -3866,7 +3872,7 @@
       <c r="E108" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="F108" s="11" t="s">
+      <c r="F108" s="10" t="s">
         <v>8</v>
       </c>
       <c r="G108" s="3"/>
@@ -3876,7 +3882,7 @@
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="B109" s="14" t="s">
+      <c r="B109" s="13" t="s">
         <v>156</v>
       </c>
       <c r="C109" s="3" t="s">
@@ -3888,7 +3894,7 @@
       <c r="E109" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="F109" s="11" t="s">
+      <c r="F109" s="10" t="s">
         <v>64</v>
       </c>
       <c r="G109" s="3"/>
@@ -3898,7 +3904,7 @@
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
-      <c r="B110" s="14" t="s">
+      <c r="B110" s="13" t="s">
         <v>157</v>
       </c>
       <c r="C110" s="3" t="s">
@@ -3910,86 +3916,86 @@
       <c r="E110" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="F110" s="11" t="s">
+      <c r="F110" s="10" t="s">
         <v>36</v>
       </c>
       <c r="G110" s="3"/>
     </row>
     <row r="111" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
-      <c r="B111" s="21"/>
-      <c r="C111" s="22"/>
-      <c r="D111" s="22"/>
-      <c r="E111" s="22"/>
-      <c r="F111" s="22"/>
+      <c r="B111" s="20"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="21"/>
+      <c r="E111" s="21"/>
+      <c r="F111" s="21"/>
       <c r="G111" s="3"/>
     </row>
     <row r="112" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
-      <c r="B112" s="21"/>
-      <c r="C112" s="22"/>
-      <c r="D112" s="22"/>
-      <c r="E112" s="22"/>
-      <c r="F112" s="22"/>
+      <c r="B112" s="20"/>
+      <c r="C112" s="21"/>
+      <c r="D112" s="21"/>
+      <c r="E112" s="21"/>
+      <c r="F112" s="21"/>
       <c r="G112" s="3"/>
     </row>
     <row r="113" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
-      <c r="B113" s="21"/>
-      <c r="C113" s="22"/>
-      <c r="D113" s="22"/>
-      <c r="E113" s="22"/>
-      <c r="F113" s="22"/>
+      <c r="B113" s="20"/>
+      <c r="C113" s="21"/>
+      <c r="D113" s="21"/>
+      <c r="E113" s="21"/>
+      <c r="F113" s="21"/>
       <c r="G113" s="3"/>
     </row>
     <row r="114" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
-      <c r="B114" s="21"/>
-      <c r="C114" s="22"/>
-      <c r="D114" s="22"/>
-      <c r="E114" s="22"/>
-      <c r="F114" s="22"/>
+      <c r="B114" s="20"/>
+      <c r="C114" s="21"/>
+      <c r="D114" s="21"/>
+      <c r="E114" s="21"/>
+      <c r="F114" s="21"/>
       <c r="G114" s="3"/>
     </row>
     <row r="115" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
-      <c r="B115" s="21"/>
-      <c r="C115" s="22"/>
-      <c r="D115" s="22"/>
-      <c r="E115" s="22"/>
-      <c r="F115" s="22"/>
+      <c r="B115" s="20"/>
+      <c r="C115" s="21"/>
+      <c r="D115" s="21"/>
+      <c r="E115" s="21"/>
+      <c r="F115" s="21"/>
       <c r="G115" s="3"/>
     </row>
     <row r="116" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
-      <c r="B116" s="21"/>
-      <c r="C116" s="22"/>
-      <c r="D116" s="22"/>
-      <c r="E116" s="22"/>
-      <c r="F116" s="22"/>
+      <c r="B116" s="20"/>
+      <c r="C116" s="21"/>
+      <c r="D116" s="21"/>
+      <c r="E116" s="21"/>
+      <c r="F116" s="21"/>
       <c r="G116" s="3"/>
     </row>
     <row r="117" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
-      <c r="B117" s="21"/>
-      <c r="C117" s="22"/>
-      <c r="D117" s="22"/>
-      <c r="E117" s="22"/>
-      <c r="F117" s="22"/>
+      <c r="B117" s="20"/>
+      <c r="C117" s="21"/>
+      <c r="D117" s="21"/>
+      <c r="E117" s="21"/>
+      <c r="F117" s="21"/>
       <c r="G117" s="3"/>
     </row>
     <row r="118" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
-      <c r="B118" s="21"/>
-      <c r="C118" s="22"/>
-      <c r="D118" s="22"/>
-      <c r="E118" s="22"/>
-      <c r="F118" s="22"/>
+      <c r="B118" s="20"/>
+      <c r="C118" s="21"/>
+      <c r="D118" s="21"/>
+      <c r="E118" s="21"/>
+      <c r="F118" s="21"/>
       <c r="G118" s="3"/>
     </row>
     <row r="119" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
-      <c r="B119" s="17"/>
+      <c r="B119" s="16"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
@@ -4001,11 +4007,11 @@
     <row r="126" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="D126" s="8"/>
       <c r="E126" s="8"/>
-      <c r="F126" s="10"/>
+      <c r="F126" s="9"/>
     </row>
     <row r="129" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
       <c r="E129" s="8"/>
-      <c r="F129" s="10"/>
+      <c r="F129" s="9"/>
     </row>
     <row r="133" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="D133" s="8"/>
@@ -4030,7 +4036,7 @@
   </sheetData>
   <autoFilter ref="F2:F121" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Ghana Maala edits - 28/07/2022
</commit_message>
<xml_diff>
--- a/Ghana Maala/Ghana Maala Content.xlsx
+++ b/Ghana Maala/Ghana Maala Content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\Ghana Maala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CD1574-9A97-43E8-990E-A5A59159863E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABD92EC-B7DB-4530-AA24-DA6C3A9D950A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1527,7 +1527,7 @@
   <dimension ref="A2:G143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="E41" sqref="E41:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2399,10 +2399,10 @@
       <c r="D41" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="26" t="s">
         <v>185</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="7" t="s">
         <v>183</v>
       </c>
       <c r="G41" s="3"/>
@@ -3213,10 +3213,10 @@
       <c r="D78" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E78" s="3" t="s">
+      <c r="E78" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="F78" s="10" t="s">
+      <c r="F78" s="7" t="s">
         <v>32</v>
       </c>
       <c r="G78" s="3"/>
@@ -3693,10 +3693,10 @@
       <c r="D100" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E100" s="3" t="s">
+      <c r="E100" s="26" t="s">
         <v>269</v>
       </c>
-      <c r="F100" s="10" t="s">
+      <c r="F100" s="7" t="s">
         <v>25</v>
       </c>
       <c r="G100" s="3"/>

</xml_diff>

<commit_message>
Ghana Maala and TS Ghanam changes
</commit_message>
<xml_diff>
--- a/Ghana Maala/Ghana Maala Content.xlsx
+++ b/Ghana Maala/Ghana Maala Content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\Ghana Maala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABD92EC-B7DB-4530-AA24-DA6C3A9D950A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC1C4CA-FAD9-41FD-BB16-249CE29A47F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,9 +121,6 @@
     <t>ahirasi buddhniyO raudrENAnIkEna</t>
   </si>
   <si>
-    <t>tAm mithunE paSyan</t>
-  </si>
-  <si>
     <t>ya evaM vidvAnagniM cinu@tE</t>
   </si>
   <si>
@@ -974,6 +971,9 @@
   </si>
   <si>
     <t>5.7.4.3</t>
+  </si>
+  <si>
+    <t>tAm mithunE apaSyan</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1185,6 +1185,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1527,7 +1530,7 @@
   <dimension ref="A2:G143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:F41"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,16 +1547,16 @@
     <row r="2" spans="1:7" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>0</v>
@@ -1567,16 +1570,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>2</v>
@@ -1589,19 +1592,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -1611,19 +1614,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -1636,16 +1639,16 @@
         <v>1.4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -1658,16 +1661,16 @@
         <v>1.5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>218</v>
+        <v>84</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>217</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -1680,16 +1683,16 @@
         <v>1.6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -1702,13 +1705,13 @@
         <v>1.7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>10</v>
@@ -1724,16 +1727,16 @@
         <v>1.8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10" s="3"/>
     </row>
@@ -1746,16 +1749,16 @@
         <v>1.9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G11" s="3"/>
     </row>
@@ -1765,16 +1768,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>218</v>
+        <v>84</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>217</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>12</v>
@@ -1787,19 +1790,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E13" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>170</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>171</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -1809,19 +1812,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G14" s="3"/>
     </row>
@@ -1831,19 +1834,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G15" s="3"/>
     </row>
@@ -1853,19 +1856,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -1875,19 +1878,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G17" s="3"/>
     </row>
@@ -1900,16 +1903,16 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E18" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>168</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>169</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -1919,19 +1922,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="3"/>
     </row>
@@ -1941,19 +1944,19 @@
         <v>18</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E20" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F20" s="11" t="s">
         <v>176</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>177</v>
       </c>
       <c r="G20" s="3"/>
     </row>
@@ -1963,19 +1966,19 @@
         <v>19</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G21" s="3"/>
     </row>
@@ -1985,19 +1988,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G22" s="3"/>
     </row>
@@ -2007,18 +2010,18 @@
         <v>21</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="F23" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="F23" s="28" t="s">
         <v>24</v>
       </c>
       <c r="G23" s="3"/>
@@ -2029,19 +2032,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G24" s="3"/>
     </row>
@@ -2051,19 +2054,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G25" s="3"/>
     </row>
@@ -2073,19 +2076,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G26" s="3"/>
     </row>
@@ -2095,19 +2098,19 @@
         <v>25</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G27" s="3"/>
     </row>
@@ -2117,19 +2120,19 @@
         <v>26</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G28" s="3"/>
     </row>
@@ -2139,19 +2142,19 @@
         <v>27</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G29" s="3"/>
     </row>
@@ -2161,19 +2164,19 @@
         <v>28</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G30" s="3"/>
     </row>
@@ -2186,16 +2189,16 @@
         <v>1.29</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G31" s="3"/>
     </row>
@@ -2205,19 +2208,19 @@
         <v>30</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G32" s="3"/>
     </row>
@@ -2230,16 +2233,16 @@
         <v>1.31</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G33" s="3"/>
     </row>
@@ -2254,10 +2257,10 @@
       <c r="C34" s="18"/>
       <c r="D34" s="3"/>
       <c r="E34" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G34" s="3"/>
     </row>
@@ -2267,19 +2270,19 @@
         <v>33</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G35" s="3"/>
     </row>
@@ -2289,19 +2292,19 @@
         <v>34</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G36" s="3"/>
     </row>
@@ -2316,10 +2319,10 @@
       <c r="C37" s="18"/>
       <c r="D37" s="3"/>
       <c r="E37" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G37" s="3"/>
     </row>
@@ -2334,10 +2337,10 @@
       <c r="C38" s="18"/>
       <c r="D38" s="3"/>
       <c r="E38" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G38" s="3"/>
     </row>
@@ -2350,16 +2353,16 @@
         <v>1.37</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G39" s="3"/>
     </row>
@@ -2372,16 +2375,16 @@
         <v>1.38</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="F40" s="10" t="s">
-        <v>59</v>
+        <v>100</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="G40" s="3"/>
     </row>
@@ -2394,16 +2397,16 @@
         <v>1.39</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G41" s="3"/>
     </row>
@@ -2413,19 +2416,19 @@
         <v>40</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E42" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="F42" s="28" t="s">
         <v>174</v>
-      </c>
-      <c r="F42" s="28" t="s">
-        <v>175</v>
       </c>
       <c r="G42" s="3"/>
     </row>
@@ -2438,13 +2441,13 @@
         <v>1.41</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F43" s="27" t="s">
         <v>13</v>
@@ -2460,16 +2463,16 @@
         <v>1.42</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G44" s="3"/>
     </row>
@@ -2482,16 +2485,16 @@
         <v>1.43</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E45" s="26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G45" s="3"/>
     </row>
@@ -2504,16 +2507,16 @@
         <v>1.44</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E46" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="F46" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="G46" s="3"/>
     </row>
@@ -2526,16 +2529,16 @@
         <v>1.45</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E47" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="F47" s="10" t="s">
         <v>208</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>209</v>
       </c>
       <c r="G47" s="3"/>
     </row>
@@ -2548,16 +2551,16 @@
         <v>1.46</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D48" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E48" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="F48" s="7" t="s">
         <v>199</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>200</v>
       </c>
       <c r="G48" s="3"/>
     </row>
@@ -2570,16 +2573,16 @@
         <v>1.47</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E49" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="G49" s="3"/>
     </row>
@@ -2589,19 +2592,19 @@
         <v>48</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>61</v>
+        <v>101</v>
+      </c>
+      <c r="E50" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="F50" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="G50" s="3"/>
     </row>
@@ -2611,19 +2614,19 @@
         <v>49</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>58</v>
+        <v>99</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="G51" s="3"/>
     </row>
@@ -2633,19 +2636,19 @@
         <v>50</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E52" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="F52" s="11" t="s">
         <v>210</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>211</v>
       </c>
       <c r="G52" s="3"/>
     </row>
@@ -2655,19 +2658,19 @@
         <v>51</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G53" s="3"/>
     </row>
@@ -2677,19 +2680,19 @@
         <v>52</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G54" s="3"/>
     </row>
@@ -2699,19 +2702,19 @@
         <v>53</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G55" s="3"/>
     </row>
@@ -2721,19 +2724,19 @@
         <v>54</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G56" s="3"/>
     </row>
@@ -2746,16 +2749,16 @@
         <v>1.55</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G57" s="3"/>
     </row>
@@ -2765,19 +2768,19 @@
         <v>56</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G58" s="3"/>
     </row>
@@ -2787,19 +2790,19 @@
         <v>57</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G59" s="3"/>
     </row>
@@ -2809,19 +2812,19 @@
         <v>58</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E60" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>201</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>202</v>
       </c>
       <c r="G60" s="3"/>
     </row>
@@ -2834,16 +2837,16 @@
         <v>1.59</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G61" s="3"/>
     </row>
@@ -2853,19 +2856,19 @@
         <v>60</v>
       </c>
       <c r="B62" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="C62" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D62" s="22" t="s">
-        <v>292</v>
-      </c>
       <c r="E62" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="F62" s="10" t="s">
         <v>178</v>
-      </c>
-      <c r="F62" s="10" t="s">
-        <v>179</v>
       </c>
       <c r="G62" s="3"/>
     </row>
@@ -2875,19 +2878,19 @@
         <v>61</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G63" s="3"/>
     </row>
@@ -2897,19 +2900,19 @@
         <v>62</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G64" s="3"/>
     </row>
@@ -2919,19 +2922,19 @@
         <v>63</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E65" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F65" s="10" t="s">
         <v>180</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>181</v>
       </c>
       <c r="G65" s="3"/>
     </row>
@@ -2944,16 +2947,16 @@
         <v>1.64</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E66" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G66" s="3"/>
     </row>
@@ -2966,13 +2969,13 @@
         <v>1.65</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E67" s="19" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F67" s="10" t="s">
         <v>17</v>
@@ -2988,16 +2991,16 @@
         <v>1.66</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G68" s="3"/>
     </row>
@@ -3010,16 +3013,16 @@
         <v>1.67</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G69" s="3"/>
     </row>
@@ -3032,16 +3035,16 @@
         <v>1.68</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G70" s="3"/>
     </row>
@@ -3054,16 +3057,16 @@
         <v>1.69</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G71" s="3"/>
     </row>
@@ -3073,19 +3076,19 @@
         <v>70</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G72" s="3"/>
     </row>
@@ -3098,16 +3101,16 @@
         <v>1.71</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G73" s="3"/>
     </row>
@@ -3117,16 +3120,16 @@
         <v>72</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F74" s="10" t="s">
         <v>6</v>
@@ -3139,16 +3142,16 @@
         <v>73</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E75" s="26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>27</v>
@@ -3164,13 +3167,13 @@
         <v>1.74</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F76" s="10" t="s">
         <v>7</v>
@@ -3183,16 +3186,16 @@
         <v>75</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F77" s="10" t="s">
         <v>9</v>
@@ -3205,19 +3208,19 @@
         <v>76</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G78" s="3"/>
     </row>
@@ -3227,16 +3230,16 @@
         <v>77</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F79" s="10" t="s">
         <v>16</v>
@@ -3249,16 +3252,16 @@
         <v>78</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F80" s="10" t="s">
         <v>14</v>
@@ -3271,16 +3274,16 @@
         <v>79</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>26</v>
@@ -3293,19 +3296,19 @@
         <v>80</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G82" s="3"/>
     </row>
@@ -3315,17 +3318,17 @@
         <v>81</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F83" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>187</v>
       </c>
       <c r="G83" s="3"/>
     </row>
@@ -3335,17 +3338,17 @@
         <v>82</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="F84" s="10" t="s">
         <v>212</v>
-      </c>
-      <c r="F84" s="10" t="s">
-        <v>213</v>
       </c>
       <c r="G84" s="3"/>
     </row>
@@ -3355,19 +3358,19 @@
         <v>83</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F85" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G85" s="3"/>
     </row>
@@ -3377,16 +3380,16 @@
         <v>84</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F86" s="10" t="s">
         <v>3</v>
@@ -3399,16 +3402,16 @@
         <v>85</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F87" s="10" t="s">
         <v>4</v>
@@ -3421,19 +3424,19 @@
         <v>86</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G88" s="3"/>
     </row>
@@ -3443,16 +3446,16 @@
         <v>87</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E89" s="26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>11</v>
@@ -3465,19 +3468,19 @@
         <v>88</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G90" s="3"/>
     </row>
@@ -3487,16 +3490,16 @@
         <v>89</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F91" s="10" t="s">
         <v>18</v>
@@ -3509,16 +3512,16 @@
         <v>90</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F92" s="10" t="s">
         <v>19</v>
@@ -3531,16 +3534,16 @@
         <v>91</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F93" s="10" t="s">
         <v>20</v>
@@ -3553,16 +3556,16 @@
         <v>92</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F94" s="10" t="s">
         <v>15</v>
@@ -3575,19 +3578,19 @@
         <v>93</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G95" s="3"/>
     </row>
@@ -3597,18 +3600,18 @@
         <v>94</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="F96" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E96" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="F96" s="28" t="s">
         <v>22</v>
       </c>
       <c r="G96" s="3"/>
@@ -3619,18 +3622,18 @@
         <v>95</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="F97" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E97" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="F97" s="28" t="s">
         <v>23</v>
       </c>
       <c r="G97" s="3"/>
@@ -3641,16 +3644,16 @@
         <v>96</v>
       </c>
       <c r="B98" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F98" s="10" t="s">
         <v>21</v>
@@ -3663,19 +3666,19 @@
         <v>97</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E99" s="25" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G99" s="3"/>
     </row>
@@ -3685,16 +3688,16 @@
         <v>98</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E100" s="26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F100" s="7" t="s">
         <v>25</v>
@@ -3706,20 +3709,20 @@
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="B101" s="13" t="s">
-        <v>151</v>
+      <c r="B101" s="29" t="s">
+        <v>150</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E101" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="F101" s="10" t="s">
-        <v>28</v>
+        <v>82</v>
+      </c>
+      <c r="E101" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>312</v>
       </c>
       <c r="G101" s="3"/>
     </row>
@@ -3729,19 +3732,19 @@
         <v>100</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F102" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G102" s="3"/>
     </row>
@@ -3751,19 +3754,19 @@
         <v>101</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F103" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G103" s="3"/>
     </row>
@@ -3773,19 +3776,19 @@
         <v>102</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F104" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G104" s="3"/>
     </row>
@@ -3795,19 +3798,19 @@
         <v>103</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F105" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G105" s="3"/>
     </row>
@@ -3817,19 +3820,19 @@
         <v>104</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E106" s="19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F106" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G106" s="3"/>
     </row>
@@ -3839,16 +3842,16 @@
         <v>105</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F107" s="10" t="s">
         <v>5</v>
@@ -3861,16 +3864,16 @@
         <v>106</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F108" s="10" t="s">
         <v>8</v>
@@ -3883,19 +3886,19 @@
         <v>107</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F109" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G109" s="3"/>
     </row>
@@ -3905,19 +3908,19 @@
         <v>108</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F110" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G110" s="3"/>
     </row>

</xml_diff>

<commit_message>
TU Files final plus Ghana MAlaa - 31/07/2022
</commit_message>
<xml_diff>
--- a/Ghana Maala/Ghana Maala Content.xlsx
+++ b/Ghana Maala/Ghana Maala Content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\Ghana Maala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC1C4CA-FAD9-41FD-BB16-249CE29A47F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8B5A24-6434-41D6-A0E6-F57E68630C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,9 +493,6 @@
     <t>2.1.</t>
   </si>
   <si>
-    <t>2.2.</t>
-  </si>
-  <si>
     <t>2.16.</t>
   </si>
   <si>
@@ -974,13 +971,16 @@
   </si>
   <si>
     <t>tAm mithunE apaSyan</t>
+  </si>
+  <si>
+    <t>1.77.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1009,6 +1009,13 @@
     </font>
     <font>
       <sz val="18"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1106,7 +1113,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1188,6 +1195,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1529,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,7 +1566,7 @@
         <v>81</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>0</v>
@@ -1578,8 +1588,8 @@
       <c r="D3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>214</v>
+      <c r="E3" s="26" t="s">
+        <v>213</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>2</v>
@@ -1601,7 +1611,7 @@
         <v>102</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>64</v>
@@ -1623,7 +1633,7 @@
         <v>84</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>73</v>
@@ -1645,7 +1655,7 @@
         <v>84</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>74</v>
@@ -1667,7 +1677,7 @@
         <v>84</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>75</v>
@@ -1689,7 +1699,7 @@
         <v>84</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>65</v>
@@ -1711,7 +1721,7 @@
         <v>84</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>10</v>
@@ -1733,7 +1743,7 @@
         <v>84</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>66</v>
@@ -1755,7 +1765,7 @@
         <v>84</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>67</v>
@@ -1777,7 +1787,7 @@
         <v>84</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>12</v>
@@ -1799,10 +1809,10 @@
         <v>84</v>
       </c>
       <c r="E13" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>169</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>170</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -1821,7 +1831,7 @@
         <v>84</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>68</v>
@@ -1843,7 +1853,7 @@
         <v>84</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>69</v>
@@ -1856,7 +1866,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>77</v>
@@ -1865,7 +1875,7 @@
         <v>84</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>72</v>
@@ -1887,7 +1897,7 @@
         <v>94</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>51</v>
@@ -1909,10 +1919,10 @@
         <v>94</v>
       </c>
       <c r="E18" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>167</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>168</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -1931,7 +1941,7 @@
         <v>94</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>52</v>
@@ -1953,10 +1963,10 @@
         <v>102</v>
       </c>
       <c r="E20" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F20" s="11" t="s">
         <v>175</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>176</v>
       </c>
       <c r="G20" s="3"/>
     </row>
@@ -1975,7 +1985,7 @@
         <v>102</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>61</v>
@@ -1997,7 +2007,7 @@
         <v>102</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>62</v>
@@ -2019,7 +2029,7 @@
         <v>87</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F23" s="28" t="s">
         <v>24</v>
@@ -2041,7 +2051,7 @@
         <v>87</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>59</v>
@@ -2063,7 +2073,7 @@
         <v>103</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>29</v>
@@ -2085,7 +2095,7 @@
         <v>82</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>40</v>
@@ -2107,7 +2117,7 @@
         <v>92</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>48</v>
@@ -2128,8 +2138,8 @@
       <c r="D28" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>231</v>
+      <c r="E28" s="30" t="s">
+        <v>230</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>49</v>
@@ -2150,10 +2160,10 @@
       <c r="D29" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="F29" s="10" t="s">
+      <c r="E29" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>47</v>
       </c>
       <c r="G29" s="3"/>
@@ -2173,10 +2183,10 @@
         <v>92</v>
       </c>
       <c r="E30" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G30" s="3"/>
     </row>
@@ -2195,10 +2205,10 @@
         <v>93</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G31" s="3"/>
     </row>
@@ -2217,7 +2227,7 @@
         <v>93</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>50</v>
@@ -2239,10 +2249,10 @@
         <v>93</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G33" s="3"/>
     </row>
@@ -2257,10 +2267,10 @@
       <c r="C34" s="18"/>
       <c r="D34" s="3"/>
       <c r="E34" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G34" s="3"/>
     </row>
@@ -2279,7 +2289,7 @@
         <v>92</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>33</v>
@@ -2301,7 +2311,7 @@
         <v>92</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>34</v>
@@ -2319,10 +2329,10 @@
       <c r="C37" s="18"/>
       <c r="D37" s="3"/>
       <c r="E37" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G37" s="3"/>
     </row>
@@ -2337,10 +2347,10 @@
       <c r="C38" s="18"/>
       <c r="D38" s="3"/>
       <c r="E38" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G38" s="3"/>
     </row>
@@ -2359,7 +2369,7 @@
         <v>100</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>30</v>
@@ -2381,7 +2391,7 @@
         <v>100</v>
       </c>
       <c r="E40" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>58</v>
@@ -2403,10 +2413,10 @@
         <v>100</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G41" s="3"/>
     </row>
@@ -2419,16 +2429,16 @@
         <v>136</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E42" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="F42" s="28" t="s">
         <v>173</v>
-      </c>
-      <c r="F42" s="28" t="s">
-        <v>174</v>
       </c>
       <c r="G42" s="3"/>
     </row>
@@ -2447,7 +2457,7 @@
         <v>85</v>
       </c>
       <c r="E43" s="26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F43" s="27" t="s">
         <v>13</v>
@@ -2469,7 +2479,7 @@
         <v>85</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>45</v>
@@ -2491,7 +2501,7 @@
         <v>85</v>
       </c>
       <c r="E45" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>46</v>
@@ -2513,10 +2523,10 @@
         <v>85</v>
       </c>
       <c r="E46" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="F46" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="G46" s="3"/>
     </row>
@@ -2535,10 +2545,10 @@
         <v>85</v>
       </c>
       <c r="E47" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="F47" s="10" t="s">
         <v>207</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>208</v>
       </c>
       <c r="G47" s="3"/>
     </row>
@@ -2557,10 +2567,10 @@
         <v>85</v>
       </c>
       <c r="E48" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="F48" s="7" t="s">
         <v>198</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>199</v>
       </c>
       <c r="G48" s="3"/>
     </row>
@@ -2579,10 +2589,10 @@
         <v>85</v>
       </c>
       <c r="E49" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>205</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>206</v>
       </c>
       <c r="G49" s="3"/>
     </row>
@@ -2601,7 +2611,7 @@
         <v>101</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F50" s="28" t="s">
         <v>60</v>
@@ -2623,7 +2633,7 @@
         <v>99</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>57</v>
@@ -2645,10 +2655,10 @@
         <v>99</v>
       </c>
       <c r="E52" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F52" s="11" t="s">
         <v>209</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>210</v>
       </c>
       <c r="G52" s="3"/>
     </row>
@@ -2658,7 +2668,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>77</v>
@@ -2667,7 +2677,7 @@
         <v>95</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>53</v>
@@ -2680,7 +2690,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>77</v>
@@ -2689,10 +2699,10 @@
         <v>95</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G54" s="3"/>
     </row>
@@ -2702,7 +2712,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>77</v>
@@ -2711,7 +2721,7 @@
         <v>97</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>55</v>
@@ -2724,7 +2734,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>77</v>
@@ -2733,7 +2743,7 @@
         <v>96</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>54</v>
@@ -2755,10 +2765,10 @@
         <v>96</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G57" s="3"/>
     </row>
@@ -2768,7 +2778,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>77</v>
@@ -2777,7 +2787,7 @@
         <v>98</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F58" s="10" t="s">
         <v>56</v>
@@ -2790,19 +2800,19 @@
         <v>57</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G59" s="3"/>
     </row>
@@ -2812,19 +2822,19 @@
         <v>58</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C60" s="22" t="s">
         <v>77</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E60" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F60" s="7" t="s">
         <v>200</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>201</v>
       </c>
       <c r="G60" s="3"/>
     </row>
@@ -2840,13 +2850,13 @@
         <v>77</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G61" s="3"/>
     </row>
@@ -2856,19 +2866,19 @@
         <v>60</v>
       </c>
       <c r="B62" s="23" t="s">
+        <v>289</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" s="22" t="s">
         <v>290</v>
       </c>
-      <c r="C62" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D62" s="22" t="s">
-        <v>291</v>
-      </c>
       <c r="E62" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F62" s="10" t="s">
         <v>177</v>
-      </c>
-      <c r="F62" s="10" t="s">
-        <v>178</v>
       </c>
       <c r="G62" s="3"/>
     </row>
@@ -2878,19 +2888,19 @@
         <v>61</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C63" s="22" t="s">
         <v>77</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G63" s="3"/>
     </row>
@@ -2900,19 +2910,19 @@
         <v>62</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C64" s="22" t="s">
         <v>77</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E64" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G64" s="3"/>
     </row>
@@ -2922,19 +2932,19 @@
         <v>63</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C65" s="22" t="s">
         <v>77</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E65" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="F65" s="10" t="s">
         <v>179</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>180</v>
       </c>
       <c r="G65" s="3"/>
     </row>
@@ -2950,13 +2960,13 @@
         <v>77</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E66" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G66" s="3"/>
     </row>
@@ -2972,10 +2982,10 @@
         <v>77</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E67" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F67" s="10" t="s">
         <v>17</v>
@@ -2997,7 +3007,7 @@
         <v>90</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F68" s="10" t="s">
         <v>44</v>
@@ -3019,7 +3029,7 @@
         <v>86</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F69" s="10" t="s">
         <v>41</v>
@@ -3041,7 +3051,7 @@
         <v>86</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F70" s="10" t="s">
         <v>42</v>
@@ -3063,7 +3073,7 @@
         <v>86</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F71" s="10" t="s">
         <v>43</v>
@@ -3076,7 +3086,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>77</v>
@@ -3085,7 +3095,7 @@
         <v>86</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F72" s="10" t="s">
         <v>70</v>
@@ -3107,7 +3117,7 @@
         <v>86</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F73" s="10" t="s">
         <v>71</v>
@@ -3120,7 +3130,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>79</v>
@@ -3129,7 +3139,7 @@
         <v>83</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F74" s="10" t="s">
         <v>6</v>
@@ -3142,7 +3152,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>80</v>
@@ -3151,7 +3161,7 @@
         <v>82</v>
       </c>
       <c r="E75" s="26" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F75" s="7" t="s">
         <v>27</v>
@@ -3172,8 +3182,8 @@
       <c r="D76" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E76" s="3" t="s">
-        <v>251</v>
+      <c r="E76" s="30" t="s">
+        <v>250</v>
       </c>
       <c r="F76" s="10" t="s">
         <v>7</v>
@@ -3186,7 +3196,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>80</v>
@@ -3195,7 +3205,7 @@
         <v>78</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F77" s="10" t="s">
         <v>9</v>
@@ -3208,7 +3218,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>80</v>
@@ -3217,7 +3227,7 @@
         <v>82</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F78" s="7" t="s">
         <v>31</v>
@@ -3229,8 +3239,8 @@
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="B79" s="13" t="s">
-        <v>305</v>
+      <c r="B79" s="29" t="s">
+        <v>304</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>80</v>
@@ -3238,8 +3248,8 @@
       <c r="D79" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E79" s="3" t="s">
-        <v>254</v>
+      <c r="E79" s="26" t="s">
+        <v>253</v>
       </c>
       <c r="F79" s="10" t="s">
         <v>16</v>
@@ -3252,7 +3262,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>80</v>
@@ -3260,8 +3270,8 @@
       <c r="D80" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E80" s="3" t="s">
-        <v>255</v>
+      <c r="E80" s="30" t="s">
+        <v>254</v>
       </c>
       <c r="F80" s="10" t="s">
         <v>14</v>
@@ -3274,7 +3284,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>80</v>
@@ -3283,7 +3293,7 @@
         <v>82</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>26</v>
@@ -3296,7 +3306,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>80</v>
@@ -3305,7 +3315,7 @@
         <v>78</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F82" s="10" t="s">
         <v>28</v>
@@ -3318,17 +3328,17 @@
         <v>81</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F83" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>186</v>
       </c>
       <c r="G83" s="3"/>
     </row>
@@ -3338,17 +3348,17 @@
         <v>82</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="F84" s="10" t="s">
         <v>211</v>
-      </c>
-      <c r="F84" s="10" t="s">
-        <v>212</v>
       </c>
       <c r="G84" s="3"/>
     </row>
@@ -3367,7 +3377,7 @@
         <v>82</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F85" s="10" t="s">
         <v>32</v>
@@ -3389,7 +3399,7 @@
         <v>82</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F86" s="10" t="s">
         <v>3</v>
@@ -3401,8 +3411,8 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="B87" s="13" t="s">
-        <v>152</v>
+      <c r="B87" s="29" t="s">
+        <v>312</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>78</v>
@@ -3410,10 +3420,10 @@
       <c r="D87" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E87" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="F87" s="10" t="s">
+      <c r="E87" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="F87" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G87" s="3"/>
@@ -3433,10 +3443,10 @@
         <v>82</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G88" s="3"/>
     </row>
@@ -3455,7 +3465,7 @@
         <v>82</v>
       </c>
       <c r="E89" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F89" s="7" t="s">
         <v>11</v>
@@ -3477,10 +3487,10 @@
         <v>82</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G90" s="3"/>
     </row>
@@ -3499,7 +3509,7 @@
         <v>82</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F91" s="10" t="s">
         <v>18</v>
@@ -3520,10 +3530,10 @@
       <c r="D92" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E92" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="F92" s="10" t="s">
+      <c r="E92" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="F92" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G92" s="3"/>
@@ -3542,10 +3552,10 @@
       <c r="D93" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E93" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="F93" s="10" t="s">
+      <c r="E93" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="F93" s="28" t="s">
         <v>20</v>
       </c>
       <c r="G93" s="3"/>
@@ -3565,7 +3575,7 @@
         <v>82</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F94" s="10" t="s">
         <v>15</v>
@@ -3587,10 +3597,10 @@
         <v>82</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G95" s="3"/>
     </row>
@@ -3609,7 +3619,7 @@
         <v>82</v>
       </c>
       <c r="E96" s="26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F96" s="28" t="s">
         <v>22</v>
@@ -3631,7 +3641,7 @@
         <v>82</v>
       </c>
       <c r="E97" s="26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F97" s="28" t="s">
         <v>23</v>
@@ -3653,7 +3663,7 @@
         <v>82</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F98" s="10" t="s">
         <v>21</v>
@@ -3675,10 +3685,10 @@
         <v>82</v>
       </c>
       <c r="E99" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G99" s="3"/>
     </row>
@@ -3697,7 +3707,7 @@
         <v>82</v>
       </c>
       <c r="E100" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F100" s="7" t="s">
         <v>25</v>
@@ -3719,10 +3729,10 @@
         <v>82</v>
       </c>
       <c r="E101" s="26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G101" s="3"/>
     </row>
@@ -3741,7 +3751,7 @@
         <v>89</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F102" s="10" t="s">
         <v>36</v>
@@ -3763,7 +3773,7 @@
         <v>89</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F103" s="10" t="s">
         <v>37</v>
@@ -3785,7 +3795,7 @@
         <v>89</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F104" s="10" t="s">
         <v>38</v>
@@ -3807,7 +3817,7 @@
         <v>89</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F105" s="10" t="s">
         <v>39</v>
@@ -3820,7 +3830,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>78</v>
@@ -3829,10 +3839,10 @@
         <v>82</v>
       </c>
       <c r="E106" s="19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F106" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G106" s="3"/>
     </row>
@@ -3842,7 +3852,7 @@
         <v>105</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>78</v>
@@ -3850,10 +3860,10 @@
       <c r="D107" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E107" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="F107" s="10" t="s">
+      <c r="E107" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="F107" s="28" t="s">
         <v>5</v>
       </c>
       <c r="G107" s="3"/>
@@ -3864,7 +3874,7 @@
         <v>106</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>78</v>
@@ -3872,10 +3882,10 @@
       <c r="D108" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E108" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="F108" s="10" t="s">
+      <c r="E108" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="F108" s="7" t="s">
         <v>8</v>
       </c>
       <c r="G108" s="3"/>
@@ -3886,7 +3896,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>78</v>
@@ -3895,7 +3905,7 @@
         <v>82</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F109" s="10" t="s">
         <v>63</v>
@@ -3908,7 +3918,7 @@
         <v>108</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>78</v>
@@ -3917,7 +3927,7 @@
         <v>88</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F110" s="10" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Ghana Maaka edits - 02/08/2022
</commit_message>
<xml_diff>
--- a/Ghana Maala/Ghana Maala Content.xlsx
+++ b/Ghana Maala/Ghana Maala Content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\Ghana Maala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8B5A24-6434-41D6-A0E6-F57E68630C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA33819-7988-40C8-829B-1817B7DA15F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -980,7 +980,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1009,13 +1009,6 @@
     </font>
     <font>
       <sz val="18"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1113,7 +1106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1195,9 +1188,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1539,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,7 +1622,7 @@
       <c r="D5" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="6" t="s">
         <v>215</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1654,7 +1644,7 @@
       <c r="D6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="6" t="s">
         <v>215</v>
       </c>
       <c r="F6" s="7" t="s">
@@ -1698,7 +1688,7 @@
       <c r="D8" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="6" t="s">
         <v>217</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -1720,7 +1710,7 @@
       <c r="D9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="6" t="s">
         <v>219</v>
       </c>
       <c r="F9" s="7" t="s">
@@ -1742,7 +1732,7 @@
       <c r="D10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="6" t="s">
         <v>218</v>
       </c>
       <c r="F10" s="7" t="s">
@@ -1764,7 +1754,7 @@
       <c r="D11" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="6" t="s">
         <v>218</v>
       </c>
       <c r="F11" s="7" t="s">
@@ -2138,10 +2128,10 @@
       <c r="D28" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="7" t="s">
         <v>49</v>
       </c>
       <c r="G28" s="3"/>
@@ -3182,10 +3172,10 @@
       <c r="D76" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E76" s="30" t="s">
+      <c r="E76" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="F76" s="10" t="s">
+      <c r="F76" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G76" s="3"/>
@@ -3270,10 +3260,10 @@
       <c r="D80" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E80" s="30" t="s">
+      <c r="E80" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="F80" s="10" t="s">
+      <c r="F80" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G80" s="3"/>

</xml_diff>

<commit_message>
Ghana Maala edits - 02/08/2022
</commit_message>
<xml_diff>
--- a/Ghana Maala/Ghana Maala Content.xlsx
+++ b/Ghana Maala/Ghana Maala Content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\Ghana Maala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA33819-7988-40C8-829B-1817B7DA15F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511BEF93-3F19-490E-A0D2-3B5DDD8B9EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1106,7 +1106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1188,6 +1188,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1530,7 +1533,7 @@
   <dimension ref="A2:G143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,7 +1823,7 @@
       <c r="D14" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="6" t="s">
         <v>220</v>
       </c>
       <c r="F14" s="7" t="s">
@@ -1842,7 +1845,7 @@
       <c r="D15" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="6" t="s">
         <v>220</v>
       </c>
       <c r="F15" s="7" t="s">
@@ -1864,7 +1867,7 @@
       <c r="D16" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="6" t="s">
         <v>221</v>
       </c>
       <c r="F16" s="7" t="s">
@@ -1952,10 +1955,10 @@
       <c r="D20" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="12" t="s">
         <v>175</v>
       </c>
       <c r="G20" s="3"/>
@@ -2446,7 +2449,7 @@
       <c r="D43" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E43" s="26" t="s">
+      <c r="E43" s="30" t="s">
         <v>236</v>
       </c>
       <c r="F43" s="27" t="s">
@@ -3241,7 +3244,7 @@
       <c r="E79" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="F79" s="10" t="s">
+      <c r="F79" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G79" s="3"/>

</xml_diff>

<commit_message>
TS Kramam 1.1 to 1.8 final - 02/08/2022
</commit_message>
<xml_diff>
--- a/Ghana Maala/Ghana Maala Content.xlsx
+++ b/Ghana Maala/Ghana Maala Content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\Ghana Maala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511BEF93-3F19-490E-A0D2-3B5DDD8B9EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F927D735-63B2-4A41-ABA8-27E58047F70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1532,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1977,10 +1977,10 @@
       <c r="D21" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="7" t="s">
         <v>61</v>
       </c>
       <c r="G21" s="3"/>
@@ -1999,10 +1999,10 @@
       <c r="D22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="7" t="s">
         <v>62</v>
       </c>
       <c r="G22" s="3"/>
@@ -2043,10 +2043,10 @@
       <c r="D24" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G24" s="3"/>
@@ -2065,10 +2065,10 @@
       <c r="D25" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G25" s="3"/>
@@ -2361,10 +2361,10 @@
       <c r="D39" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F39" s="7" t="s">
         <v>30</v>
       </c>
       <c r="G39" s="3"/>

</xml_diff>

<commit_message>
TS 2.6 Ghana Jatai Raja output plus Ghana Maala final - 08/08/2022
</commit_message>
<xml_diff>
--- a/Ghana Maala/Ghana Maala Content.xlsx
+++ b/Ghana Maala/Ghana Maala Content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\Ghana Maala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F927D735-63B2-4A41-ABA8-27E58047F70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84E25EF-6850-458F-A135-D2C0E3E07FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="297">
   <si>
     <t>Ghanam Description</t>
   </si>
@@ -58,9 +58,6 @@
     <t>OShadhayaH sam~Mva#dantE</t>
   </si>
   <si>
-    <t>agnir vratapa#tir vra@tamA</t>
-  </si>
-  <si>
     <t>navO navO Bavati</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>santvA si~jcAmi yajuShA</t>
   </si>
   <si>
-    <t>e@Sha tE# rudra BA@gasta~jju#Shasva</t>
-  </si>
-  <si>
     <t>idamindra pratihavyam gRuBAya</t>
   </si>
   <si>
@@ -214,9 +208,6 @@
     <t xml:space="preserve">imam mE varuna , tat tvA yAmi  </t>
   </si>
   <si>
-    <t>bra@hmA dE@vAnA$m</t>
-  </si>
-  <si>
     <t>prajApatE na tvadEtAnyanyO</t>
   </si>
   <si>
@@ -352,33 +343,9 @@
     <t>Final File</t>
   </si>
   <si>
-    <t>2.4.1</t>
-  </si>
-  <si>
-    <t>2.8.1</t>
-  </si>
-  <si>
-    <t>2.9.1</t>
-  </si>
-  <si>
     <t>2.10.</t>
   </si>
   <si>
-    <t>2.1.1</t>
-  </si>
-  <si>
-    <t>2.14.1</t>
-  </si>
-  <si>
-    <t>2.14.2</t>
-  </si>
-  <si>
-    <t>2.14.3</t>
-  </si>
-  <si>
-    <t>2.9.</t>
-  </si>
-  <si>
     <t>1.1.</t>
   </si>
   <si>
@@ -463,30 +430,9 @@
     <t>2.14.</t>
   </si>
   <si>
-    <t>2.4.</t>
-  </si>
-  <si>
-    <t>2.3.</t>
-  </si>
-  <si>
-    <t>2.8.</t>
-  </si>
-  <si>
-    <t>2.5.</t>
-  </si>
-  <si>
-    <t>2.6.</t>
-  </si>
-  <si>
-    <t>2.7.</t>
-  </si>
-  <si>
     <t>2.11.</t>
   </si>
   <si>
-    <t>2.12.</t>
-  </si>
-  <si>
     <t>2.13.</t>
   </si>
   <si>
@@ -505,9 +451,6 @@
     <t>2.19.</t>
   </si>
   <si>
-    <t>2.15.</t>
-  </si>
-  <si>
     <t>3.4.10.1</t>
   </si>
   <si>
@@ -955,25 +898,34 @@
     <t>1.78.</t>
   </si>
   <si>
-    <t>1.79.</t>
-  </si>
-  <si>
-    <t>1.80.</t>
-  </si>
-  <si>
-    <t>1.82.</t>
-  </si>
-  <si>
-    <t>1.81.</t>
-  </si>
-  <si>
     <t>5.7.4.3</t>
   </si>
   <si>
     <t>tAm mithunE apaSyan</t>
   </si>
   <si>
-    <t>1.77.1</t>
+    <t>agnir vratapa#tir vratamA</t>
+  </si>
+  <si>
+    <t>2.21.</t>
+  </si>
+  <si>
+    <t>2.20.</t>
+  </si>
+  <si>
+    <t>2.22.</t>
+  </si>
+  <si>
+    <t>2.23.</t>
+  </si>
+  <si>
+    <t>2.25.</t>
+  </si>
+  <si>
+    <t>eSha tE# rudra BA@gasta~jju#Shasva</t>
+  </si>
+  <si>
+    <t>brahmA dE@vAnA$m</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1058,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1134,9 +1086,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1158,9 +1107,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1180,16 +1126,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1532,14 +1469,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="16" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
@@ -1549,17 +1486,17 @@
   <sheetData>
     <row r="2" spans="1:7" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="14" t="s">
-        <v>104</v>
+      <c r="B2" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>0</v>
@@ -1572,17 +1509,17 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>114</v>
+      <c r="B3" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>213</v>
+        <v>79</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>194</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>2</v>
@@ -1594,20 +1531,20 @@
         <f>+A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>115</v>
+      <c r="B4" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -1616,20 +1553,20 @@
         <f t="shared" ref="A5:A110" si="0">+A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>116</v>
+      <c r="B5" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G5" s="3"/>
     </row>
@@ -1638,20 +1575,20 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>1.4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -1660,20 +1597,20 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>1.5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>216</v>
+        <v>81</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>197</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G7" s="3"/>
     </row>
@@ -1682,20 +1619,20 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>1.6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G8" s="3"/>
     </row>
@@ -1704,20 +1641,20 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="12">
         <v>1.7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" s="3"/>
     </row>
@@ -1726,20 +1663,20 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>1.8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G10" s="3"/>
     </row>
@@ -1748,20 +1685,20 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>1.9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G11" s="3"/>
     </row>
@@ -1770,20 +1707,20 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>117</v>
+      <c r="B12" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>216</v>
+        <v>81</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>197</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>12</v>
+        <v>295</v>
       </c>
       <c r="G12" s="3"/>
     </row>
@@ -1792,20 +1729,20 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>118</v>
+      <c r="B13" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>169</v>
+        <v>81</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -1814,20 +1751,20 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>119</v>
+      <c r="B14" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G14" s="3"/>
     </row>
@@ -1836,20 +1773,20 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>120</v>
+      <c r="B15" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G15" s="3"/>
     </row>
@@ -1858,20 +1795,20 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>279</v>
+      <c r="B16" s="12" t="s">
+        <v>260</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -1880,20 +1817,20 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>121</v>
+      <c r="B17" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G17" s="3"/>
     </row>
@@ -1902,20 +1839,20 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="12">
         <v>1.1599999999999999</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>167</v>
+        <v>91</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>148</v>
       </c>
       <c r="G18" s="3"/>
     </row>
@@ -1924,20 +1861,20 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>124</v>
+      <c r="B19" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G19" s="3"/>
     </row>
@@ -1946,20 +1883,20 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>123</v>
+      <c r="B20" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>175</v>
+        <v>99</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>156</v>
       </c>
       <c r="G20" s="3"/>
     </row>
@@ -1968,20 +1905,20 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>122</v>
+      <c r="B21" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G21" s="3"/>
     </row>
@@ -1990,20 +1927,20 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>126</v>
+      <c r="B22" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G22" s="3"/>
     </row>
@@ -2012,20 +1949,20 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>127</v>
+      <c r="B23" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>24</v>
+        <v>84</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="G23" s="3"/>
     </row>
@@ -2034,20 +1971,20 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>134</v>
+      <c r="B24" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>59</v>
+        <v>296</v>
       </c>
       <c r="G24" s="3"/>
     </row>
@@ -2056,20 +1993,20 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>125</v>
+      <c r="B25" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G25" s="3"/>
     </row>
@@ -2078,20 +2015,20 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>137</v>
+      <c r="B26" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G26" s="3"/>
     </row>
@@ -2100,20 +2037,20 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>128</v>
+      <c r="B27" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="26" t="s">
-        <v>229</v>
+        <v>89</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>210</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G27" s="3"/>
     </row>
@@ -2122,20 +2059,20 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>129</v>
+      <c r="B28" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>230</v>
+        <v>89</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>211</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G28" s="3"/>
     </row>
@@ -2144,20 +2081,20 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>132</v>
+      <c r="B29" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>231</v>
+        <v>88</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>212</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G29" s="3"/>
     </row>
@@ -2166,20 +2103,20 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>133</v>
+      <c r="B30" s="12" t="s">
+        <v>122</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30" s="26" t="s">
-        <v>182</v>
+        <v>89</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>163</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="G30" s="3"/>
     </row>
@@ -2188,20 +2125,20 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B31" s="12">
         <v>1.29</v>
       </c>
-      <c r="C31" s="18" t="s">
-        <v>77</v>
+      <c r="C31" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="G31" s="3"/>
     </row>
@@ -2210,20 +2147,20 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>77</v>
+      <c r="B32" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G32" s="3"/>
     </row>
@@ -2232,20 +2169,20 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B33" s="12">
         <v>1.31</v>
       </c>
-      <c r="C33" s="18" t="s">
-        <v>77</v>
+      <c r="C33" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="G33" s="3"/>
     </row>
@@ -2254,16 +2191,16 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B34" s="12">
         <v>1.32</v>
       </c>
-      <c r="C34" s="18"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="3"/>
       <c r="E34" s="6" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="G34" s="3"/>
     </row>
@@ -2272,20 +2209,20 @@
         <f>+A34+1</f>
         <v>33</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>130</v>
+      <c r="B35" s="12" t="s">
+        <v>119</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G35" s="3"/>
     </row>
@@ -2294,20 +2231,20 @@
         <f>+A35+1</f>
         <v>34</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>131</v>
+      <c r="B36" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G36" s="3"/>
     </row>
@@ -2316,16 +2253,16 @@
         <f t="shared" ref="A37:A60" si="1">+A36+1</f>
         <v>35</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="12">
         <v>1.35</v>
       </c>
-      <c r="C37" s="18"/>
+      <c r="C37" s="17"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>186</v>
+      <c r="E37" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="G37" s="3"/>
     </row>
@@ -2334,16 +2271,16 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B38" s="13">
+      <c r="B38" s="12">
         <v>1.36</v>
       </c>
-      <c r="C38" s="18"/>
+      <c r="C38" s="17"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>202</v>
+      <c r="E38" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="G38" s="3"/>
     </row>
@@ -2352,20 +2289,20 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B39" s="13">
+      <c r="B39" s="12">
         <v>1.37</v>
       </c>
-      <c r="C39" s="18" t="s">
-        <v>77</v>
+      <c r="C39" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G39" s="3"/>
     </row>
@@ -2374,20 +2311,20 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B40" s="13">
+      <c r="B40" s="12">
         <v>1.38</v>
       </c>
-      <c r="C40" s="18" t="s">
-        <v>77</v>
+      <c r="C40" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>235</v>
+        <v>97</v>
+      </c>
+      <c r="E40" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G40" s="3"/>
     </row>
@@ -2396,20 +2333,20 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B41" s="13">
+      <c r="B41" s="12">
         <v>1.39</v>
       </c>
-      <c r="C41" s="18" t="s">
-        <v>77</v>
+      <c r="C41" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E41" s="26" t="s">
-        <v>183</v>
+        <v>97</v>
+      </c>
+      <c r="E41" s="24" t="s">
+        <v>164</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="G41" s="3"/>
     </row>
@@ -2418,20 +2355,20 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B42" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>280</v>
+      <c r="B42" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>261</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E42" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="F42" s="28" t="s">
-        <v>173</v>
+        <v>82</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>154</v>
       </c>
       <c r="G42" s="3"/>
     </row>
@@ -2440,20 +2377,20 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B43" s="13">
+      <c r="B43" s="12">
         <v>1.41</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="F43" s="27" t="s">
-        <v>13</v>
+        <v>82</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="F43" s="25" t="s">
+        <v>11</v>
       </c>
       <c r="G43" s="3"/>
     </row>
@@ -2462,20 +2399,20 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B44" s="13">
+      <c r="B44" s="12">
         <v>1.42</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>45</v>
+        <v>82</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="G44" s="3"/>
     </row>
@@ -2484,350 +2421,350 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B45" s="13">
+      <c r="B45" s="12">
         <v>1.43</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E45" s="26" t="s">
-        <v>237</v>
+        <v>82</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>218</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22">
+      <c r="A46" s="20">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B46" s="23">
+      <c r="B46" s="21">
         <v>1.44</v>
       </c>
-      <c r="C46" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E46" s="26" t="s">
-        <v>161</v>
+      <c r="C46" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22">
+      <c r="A47" s="20">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B47" s="23">
+      <c r="B47" s="21">
         <v>1.45</v>
       </c>
-      <c r="C47" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E47" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>207</v>
+      <c r="C47" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22">
+      <c r="A48" s="20">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B48" s="23">
+      <c r="B48" s="21">
         <v>1.46</v>
       </c>
-      <c r="C48" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D48" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E48" s="26" t="s">
-        <v>197</v>
+      <c r="C48" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>178</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22">
+      <c r="A49" s="20">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B49" s="23">
+      <c r="B49" s="21">
         <v>1.47</v>
       </c>
-      <c r="C49" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E49" s="26" t="s">
-        <v>204</v>
+      <c r="C49" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49" s="24" t="s">
+        <v>185</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="22">
+      <c r="A50" s="20">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B50" s="13" t="s">
-        <v>139</v>
+      <c r="B50" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E50" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="F50" s="28" t="s">
-        <v>60</v>
+        <v>98</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="F50" s="25" t="s">
+        <v>57</v>
       </c>
       <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="22">
+      <c r="A51" s="20">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="B51" s="13" t="s">
-        <v>140</v>
+      <c r="B51" s="12" t="s">
+        <v>129</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E51" s="26" t="s">
-        <v>239</v>
+        <v>96</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>220</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="22">
+      <c r="A52" s="20">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B52" s="13" t="s">
-        <v>138</v>
+      <c r="B52" s="12" t="s">
+        <v>127</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>208</v>
+        <v>96</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>189</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="22">
+      <c r="A53" s="20">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="B53" s="13" t="s">
-        <v>281</v>
+      <c r="B53" s="12" t="s">
+        <v>262</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>53</v>
+        <v>92</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="G53" s="3"/>
     </row>
     <row r="54" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="22">
+      <c r="A54" s="20">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="B54" s="13" t="s">
-        <v>282</v>
+      <c r="B54" s="12" t="s">
+        <v>263</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>171</v>
+        <v>92</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>152</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="G54" s="3"/>
     </row>
     <row r="55" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="22">
+      <c r="A55" s="20">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="B55" s="13" t="s">
-        <v>283</v>
+      <c r="B55" s="12" t="s">
+        <v>264</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>55</v>
+        <v>94</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="G55" s="3"/>
     </row>
     <row r="56" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="22">
+      <c r="A56" s="20">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="B56" s="13" t="s">
-        <v>284</v>
+      <c r="B56" s="12" t="s">
+        <v>265</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>54</v>
+        <v>93</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="22">
+      <c r="A57" s="20">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="B57" s="13">
+      <c r="B57" s="12">
         <v>1.55</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="G57" s="3"/>
     </row>
     <row r="58" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="22">
+      <c r="A58" s="20">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="B58" s="13" t="s">
-        <v>286</v>
+      <c r="B58" s="12" t="s">
+        <v>267</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>56</v>
+        <v>95</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="22">
+      <c r="A59" s="20">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="B59" s="13" t="s">
-        <v>285</v>
+      <c r="B59" s="12" t="s">
+        <v>266</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>187</v>
+        <v>268</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="G59" s="3"/>
     </row>
     <row r="60" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22">
+      <c r="A60" s="20">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="B60" s="23" t="s">
-        <v>288</v>
-      </c>
-      <c r="C60" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D60" s="22" t="s">
-        <v>287</v>
+      <c r="B60" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>268</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="G60" s="3"/>
     </row>
@@ -2836,457 +2773,457 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B61" s="23">
+      <c r="B61" s="21">
         <v>1.59</v>
       </c>
-      <c r="C61" s="22" t="s">
+      <c r="C61" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G61" s="3"/>
+    </row>
+    <row r="62" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="20">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="G62" s="3"/>
+    </row>
+    <row r="63" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="20">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G63" s="3"/>
+    </row>
+    <row r="64" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="20">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="G64" s="3"/>
+    </row>
+    <row r="65" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="20">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G65" s="3"/>
+    </row>
+    <row r="66" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="20">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B66" s="12">
+        <v>1.64</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="20">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B67" s="12">
+        <v>1.65</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="20">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B68" s="12">
+        <v>1.66</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G68" s="3"/>
+    </row>
+    <row r="69" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="20">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="B69" s="12">
+        <v>1.67</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G69" s="3"/>
+    </row>
+    <row r="70" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="20">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="B70" s="12">
+        <v>1.68</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G70" s="3"/>
+    </row>
+    <row r="71" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="20">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="B71" s="12">
+        <v>1.69</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G71" s="3"/>
+    </row>
+    <row r="72" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="20">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="B72" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G72" s="3"/>
+    </row>
+    <row r="73" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="20">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="B73" s="12">
+        <v>1.71</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G73" s="3"/>
+    </row>
+    <row r="74" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="20">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="B74" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G74" s="3"/>
+    </row>
+    <row r="75" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="20">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D61" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="F61" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="G61" s="3"/>
-    </row>
-    <row r="62" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="22">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B62" s="23" t="s">
+      <c r="D75" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E75" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G75" s="3"/>
+    </row>
+    <row r="76" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="20">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="B76" s="12">
+        <v>1.74</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E76" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="F76" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="G76" s="3"/>
+    </row>
+    <row r="77" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="20">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D62" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="E62" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="F62" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="G62" s="3"/>
-    </row>
-    <row r="63" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="22">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B63" s="23" t="s">
-        <v>291</v>
-      </c>
-      <c r="C63" s="22" t="s">
+      <c r="D77" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G77" s="3"/>
+    </row>
+    <row r="78" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="20">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="G63" s="3"/>
-    </row>
-    <row r="64" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="22">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B64" s="23" t="s">
-        <v>292</v>
-      </c>
-      <c r="C64" s="22" t="s">
+      <c r="D78" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E78" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G78" s="3"/>
+    </row>
+    <row r="79" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="20">
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="E64" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="F64" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="G64" s="3"/>
-    </row>
-    <row r="65" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="22">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B65" s="23" t="s">
-        <v>293</v>
-      </c>
-      <c r="C65" s="22" t="s">
+      <c r="B79" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="E65" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="F65" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="G65" s="3"/>
-    </row>
-    <row r="66" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="22">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B66" s="13">
-        <v>1.64</v>
-      </c>
-      <c r="C66" s="22" t="s">
+      <c r="D79" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E79" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" s="3"/>
+    </row>
+    <row r="80" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="20">
+        <f t="shared" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="E66" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="F66" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="G66" s="3"/>
-    </row>
-    <row r="67" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="22">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="B67" s="13">
-        <v>1.65</v>
-      </c>
-      <c r="C67" s="3" t="s">
+      <c r="D80" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G80" s="3"/>
+    </row>
+    <row r="81" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="20">
+        <f t="shared" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="B81" s="12">
+        <v>1.79</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>310</v>
-      </c>
-      <c r="F67" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G67" s="3"/>
-    </row>
-    <row r="68" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="22">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="B68" s="13">
-        <v>1.66</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F68" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G68" s="3"/>
-    </row>
-    <row r="69" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="22">
-        <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="B69" s="13">
-        <v>1.67</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="F69" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G69" s="3"/>
-    </row>
-    <row r="70" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="22">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="B70" s="13">
-        <v>1.68</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F70" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G70" s="3"/>
-    </row>
-    <row r="71" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="22">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="B71" s="13">
-        <v>1.69</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F71" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G71" s="3"/>
-    </row>
-    <row r="72" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="22">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="B72" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="F72" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G72" s="3"/>
-    </row>
-    <row r="73" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="22">
-        <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
-      <c r="B73" s="13">
-        <v>1.71</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="F73" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="G73" s="3"/>
-    </row>
-    <row r="74" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="22">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="B74" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F74" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G74" s="3"/>
-    </row>
-    <row r="75" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="22">
-        <f t="shared" si="0"/>
-        <v>73</v>
-      </c>
-      <c r="B75" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E75" s="26" t="s">
-        <v>249</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G75" s="3"/>
-    </row>
-    <row r="76" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="22">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="B76" s="13">
-        <v>1.74</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E76" s="26" t="s">
-        <v>250</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G76" s="3"/>
-    </row>
-    <row r="77" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="22">
-        <f t="shared" si="0"/>
+      <c r="D81" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B77" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="F77" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G77" s="3"/>
-    </row>
-    <row r="78" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="22">
-        <f t="shared" si="0"/>
-        <v>76</v>
-      </c>
-      <c r="B78" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E78" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G78" s="3"/>
-    </row>
-    <row r="79" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="22">
-        <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-      <c r="B79" s="29" t="s">
-        <v>304</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E79" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G79" s="3"/>
-    </row>
-    <row r="80" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="22">
-        <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-      <c r="B80" s="13" t="s">
-        <v>305</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E80" s="26" t="s">
-        <v>254</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G80" s="3"/>
-    </row>
-    <row r="81" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-      <c r="B81" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="E81" s="6" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>26</v>
@@ -3294,127 +3231,127 @@
       <c r="G81" s="3"/>
     </row>
     <row r="82" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="3">
+      <c r="A82" s="20">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="B82" s="13" t="s">
-        <v>307</v>
+      <c r="B82" s="12">
+        <v>1.8</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="F82" s="10" t="s">
-        <v>28</v>
+        <v>77</v>
+      </c>
+      <c r="D82" s="19"/>
+      <c r="E82" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="G82" s="3"/>
     </row>
     <row r="83" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="3">
+      <c r="A83" s="20">
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="B83" s="13" t="s">
-        <v>309</v>
+      <c r="B83" s="12">
+        <v>1.81</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D83" s="21"/>
+        <v>77</v>
+      </c>
+      <c r="D83" s="19"/>
       <c r="E83" s="6" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="G83" s="3"/>
     </row>
     <row r="84" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="3">
+      <c r="A84" s="20">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="B84" s="13" t="s">
-        <v>308</v>
+      <c r="B84" s="12" t="s">
+        <v>133</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D84" s="21"/>
-      <c r="E84" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="F84" s="10" t="s">
-        <v>211</v>
+        <v>75</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="G84" s="3"/>
     </row>
     <row r="85" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="3">
+      <c r="A85" s="20">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
-      <c r="B85" s="13" t="s">
-        <v>151</v>
+      <c r="B85" s="12">
+        <v>2.2000000000000002</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="F85" s="10" t="s">
-        <v>32</v>
+        <v>79</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="G85" s="3"/>
     </row>
     <row r="86" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="3">
+      <c r="A86" s="20">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="B86" s="13" t="s">
-        <v>109</v>
+      <c r="B86" s="12">
+        <v>2.2999999999999998</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="F86" s="10" t="s">
-        <v>3</v>
+        <v>75</v>
+      </c>
+      <c r="E86" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="G86" s="3"/>
     </row>
     <row r="87" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3">
+      <c r="A87" s="20">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="B87" s="29" t="s">
-        <v>312</v>
+      <c r="B87" s="12">
+        <v>2.4</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="F87" s="7" t="s">
         <v>4</v>
@@ -3422,586 +3359,586 @@
       <c r="G87" s="3"/>
     </row>
     <row r="88" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="3">
+      <c r="A88" s="20">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
-      <c r="B88" s="13" t="s">
-        <v>143</v>
+      <c r="B88" s="12">
+        <v>2.5</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E88" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="G88" s="3"/>
+    </row>
+    <row r="89" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="20">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="B89" s="12">
+        <v>2.6</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E89" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="20">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="B90" s="12">
+        <v>2.7</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E90" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="G90" s="3"/>
+    </row>
+    <row r="91" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="20">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="B91" s="12">
+        <v>2.8</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G91" s="3"/>
+    </row>
+    <row r="92" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="20">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="B92" s="12">
+        <v>2.9</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G92" s="3"/>
+    </row>
+    <row r="93" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="20">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E93" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="F93" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G93" s="3"/>
+    </row>
+    <row r="94" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="20">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G94" s="3"/>
+    </row>
+    <row r="95" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="20">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="B95" s="12">
+        <v>2.12</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="G95" s="3"/>
+    </row>
+    <row r="96" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="20">
+        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E96" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="G96" s="3"/>
+    </row>
+    <row r="97" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="20">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E97" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="F97" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G97" s="3"/>
+    </row>
+    <row r="98" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="20">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="B98" s="12">
+        <v>2.15</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E98" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="F98" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G98" s="3"/>
+    </row>
+    <row r="99" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="20">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G99" s="3"/>
+    </row>
+    <row r="100" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="20">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E100" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="G100" s="3"/>
+    </row>
+    <row r="101" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="20">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E101" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G101" s="3"/>
+    </row>
+    <row r="102" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="20">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="B102" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G102" s="3"/>
+    </row>
+    <row r="103" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="20">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="B103" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G103" s="3"/>
+    </row>
+    <row r="104" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="20">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+      <c r="B104" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G104" s="3"/>
+    </row>
+    <row r="105" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="20">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G105" s="3"/>
+    </row>
+    <row r="106" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="20">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="B106" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="F106" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="F88" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="G88" s="3"/>
-    </row>
-    <row r="89" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="3">
-        <f t="shared" si="0"/>
-        <v>87</v>
-      </c>
-      <c r="B89" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E89" s="26" t="s">
-        <v>260</v>
-      </c>
-      <c r="F89" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G89" s="3"/>
-    </row>
-    <row r="90" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="3">
-        <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="B90" s="13" t="s">
+      <c r="G106" s="3"/>
+    </row>
+    <row r="107" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="20">
+        <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E90" s="26" t="s">
-        <v>260</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="G90" s="3"/>
-    </row>
-    <row r="91" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="3">
-        <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
-      <c r="B91" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="F91" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G91" s="3"/>
-    </row>
-    <row r="92" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="3">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="B92" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G92" s="3"/>
-    </row>
-    <row r="93" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="3">
-        <f t="shared" si="0"/>
-        <v>91</v>
-      </c>
-      <c r="B93" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E93" s="26" t="s">
-        <v>263</v>
-      </c>
-      <c r="F93" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="G93" s="3"/>
-    </row>
-    <row r="94" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="3">
-        <f t="shared" si="0"/>
-        <v>92</v>
-      </c>
-      <c r="B94" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="F94" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G94" s="3"/>
-    </row>
-    <row r="95" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="3">
-        <f t="shared" si="0"/>
-        <v>93</v>
-      </c>
-      <c r="B95" s="13" t="s">
+      <c r="B107" s="12">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E107" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="F107" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G107" s="3"/>
+    </row>
+    <row r="108" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="20">
+        <f t="shared" si="0"/>
         <v>106</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D95" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="F95" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="G95" s="3"/>
-    </row>
-    <row r="96" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="3">
-        <f t="shared" si="0"/>
-        <v>94</v>
-      </c>
-      <c r="B96" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E96" s="26" t="s">
-        <v>265</v>
-      </c>
-      <c r="F96" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G96" s="3"/>
-    </row>
-    <row r="97" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="3">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-      <c r="B97" s="13" t="s">
+      <c r="B108" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E108" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G108" s="3"/>
+    </row>
+    <row r="109" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="20">
+        <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="C97" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E97" s="26" t="s">
-        <v>265</v>
-      </c>
-      <c r="F97" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="G97" s="3"/>
-    </row>
-    <row r="98" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="3">
-        <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-      <c r="B98" s="15" t="s">
+      <c r="B109" s="12">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G109" s="3"/>
+    </row>
+    <row r="110" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="20">
+        <f t="shared" si="0"/>
         <v>108</v>
       </c>
-      <c r="C98" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D98" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="F98" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G98" s="3"/>
-    </row>
-    <row r="99" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="3">
-        <f t="shared" si="0"/>
-        <v>97</v>
-      </c>
-      <c r="B99" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E99" s="25" t="s">
-        <v>268</v>
-      </c>
-      <c r="F99" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="G99" s="3"/>
-    </row>
-    <row r="100" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="3">
-        <f t="shared" si="0"/>
-        <v>98</v>
-      </c>
-      <c r="B100" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E100" s="26" t="s">
-        <v>267</v>
-      </c>
-      <c r="F100" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G100" s="3"/>
-    </row>
-    <row r="101" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="3">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-      <c r="B101" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E101" s="26" t="s">
-        <v>265</v>
-      </c>
-      <c r="F101" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="G101" s="3"/>
-    </row>
-    <row r="102" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="3">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="B102" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="F102" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G102" s="3"/>
-    </row>
-    <row r="103" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="3">
-        <f t="shared" si="0"/>
-        <v>101</v>
-      </c>
-      <c r="B103" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="F103" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G103" s="3"/>
-    </row>
-    <row r="104" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="3">
-        <f t="shared" si="0"/>
-        <v>102</v>
-      </c>
-      <c r="B104" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="F104" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G104" s="3"/>
-    </row>
-    <row r="105" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="3">
-        <f t="shared" si="0"/>
-        <v>103</v>
-      </c>
-      <c r="B105" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="F105" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G105" s="3"/>
-    </row>
-    <row r="106" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="3">
-        <f t="shared" si="0"/>
-        <v>104</v>
-      </c>
-      <c r="B106" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E106" s="19" t="s">
-        <v>270</v>
-      </c>
-      <c r="F106" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="G106" s="3"/>
-    </row>
-    <row r="107" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="3">
-        <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-      <c r="B107" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E107" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="F107" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="G107" s="3"/>
-    </row>
-    <row r="108" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="3">
-        <f t="shared" si="0"/>
-        <v>106</v>
-      </c>
-      <c r="B108" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E108" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="F108" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G108" s="3"/>
-    </row>
-    <row r="109" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="3">
-        <f t="shared" si="0"/>
-        <v>107</v>
-      </c>
-      <c r="B109" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="F109" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G109" s="3"/>
-    </row>
-    <row r="110" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="3">
-        <f t="shared" si="0"/>
-        <v>108</v>
-      </c>
-      <c r="B110" s="13" t="s">
-        <v>155</v>
+      <c r="B110" s="12">
+        <v>2.27</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="F110" s="10" t="s">
-        <v>35</v>
+        <v>85</v>
+      </c>
+      <c r="E110" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="G110" s="3"/>
     </row>
     <row r="111" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
-      <c r="B111" s="20"/>
-      <c r="C111" s="21"/>
-      <c r="D111" s="21"/>
-      <c r="E111" s="21"/>
-      <c r="F111" s="21"/>
+      <c r="B111" s="18"/>
+      <c r="C111" s="19"/>
+      <c r="D111" s="19"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
       <c r="G111" s="3"/>
     </row>
     <row r="112" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
-      <c r="B112" s="20"/>
-      <c r="C112" s="21"/>
-      <c r="D112" s="21"/>
-      <c r="E112" s="21"/>
-      <c r="F112" s="21"/>
+      <c r="B112" s="18"/>
+      <c r="C112" s="19"/>
+      <c r="D112" s="19"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="19"/>
       <c r="G112" s="3"/>
     </row>
     <row r="113" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
-      <c r="B113" s="20"/>
-      <c r="C113" s="21"/>
-      <c r="D113" s="21"/>
-      <c r="E113" s="21"/>
-      <c r="F113" s="21"/>
+      <c r="B113" s="18"/>
+      <c r="C113" s="19"/>
+      <c r="D113" s="19"/>
+      <c r="E113" s="19"/>
+      <c r="F113" s="19"/>
       <c r="G113" s="3"/>
     </row>
     <row r="114" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
-      <c r="B114" s="20"/>
-      <c r="C114" s="21"/>
-      <c r="D114" s="21"/>
-      <c r="E114" s="21"/>
-      <c r="F114" s="21"/>
+      <c r="B114" s="18"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="19"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19"/>
       <c r="G114" s="3"/>
     </row>
     <row r="115" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
-      <c r="B115" s="20"/>
-      <c r="C115" s="21"/>
-      <c r="D115" s="21"/>
-      <c r="E115" s="21"/>
-      <c r="F115" s="21"/>
+      <c r="B115" s="18"/>
+      <c r="C115" s="19"/>
+      <c r="D115" s="19"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="19"/>
       <c r="G115" s="3"/>
     </row>
     <row r="116" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
-      <c r="B116" s="20"/>
-      <c r="C116" s="21"/>
-      <c r="D116" s="21"/>
-      <c r="E116" s="21"/>
-      <c r="F116" s="21"/>
+      <c r="B116" s="18"/>
+      <c r="C116" s="19"/>
+      <c r="D116" s="19"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="19"/>
       <c r="G116" s="3"/>
     </row>
     <row r="117" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
-      <c r="B117" s="20"/>
-      <c r="C117" s="21"/>
-      <c r="D117" s="21"/>
-      <c r="E117" s="21"/>
-      <c r="F117" s="21"/>
+      <c r="B117" s="18"/>
+      <c r="C117" s="19"/>
+      <c r="D117" s="19"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="19"/>
       <c r="G117" s="3"/>
     </row>
     <row r="118" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
-      <c r="B118" s="20"/>
-      <c r="C118" s="21"/>
-      <c r="D118" s="21"/>
-      <c r="E118" s="21"/>
-      <c r="F118" s="21"/>
+      <c r="B118" s="18"/>
+      <c r="C118" s="19"/>
+      <c r="D118" s="19"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
       <c r="G118" s="3"/>
     </row>
     <row r="119" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
-      <c r="B119" s="16"/>
+      <c r="B119" s="15"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>

</xml_diff>

<commit_message>
Ghana Maala final - incl 2.6 corr - 09/08/2022
</commit_message>
<xml_diff>
--- a/Ghana Maala/Ghana Maala Content.xlsx
+++ b/Ghana Maala/Ghana Maala Content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\Ghana Maala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84E25EF-6850-458F-A135-D2C0E3E07FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4582C3A3-6299-43E3-AE9C-847CBBAA11B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1083,9 +1083,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1127,6 +1124,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1469,14 +1469,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="15" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
@@ -1486,7 +1486,7 @@
   <sheetData>
     <row r="2" spans="1:7" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>101</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1509,7 +1509,7 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>103</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1518,7 +1518,7 @@
       <c r="D3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>194</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -1531,7 +1531,7 @@
         <f>+A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>104</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1553,7 +1553,7 @@
         <f t="shared" ref="A5:A110" si="0">+A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>105</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1575,7 +1575,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>1.4</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1597,7 +1597,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>1.5</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1606,7 +1606,7 @@
       <c r="D7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>197</v>
       </c>
       <c r="F7" s="7" t="s">
@@ -1619,7 +1619,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>1.6</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1641,7 +1641,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>1.7</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1663,7 +1663,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>1.8</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1685,7 +1685,7 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>1.9</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1707,7 +1707,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>106</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1716,7 +1716,7 @@
       <c r="D12" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>197</v>
       </c>
       <c r="F12" s="7" t="s">
@@ -1729,7 +1729,7 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>107</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1738,10 +1738,10 @@
       <c r="D13" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="10" t="s">
         <v>150</v>
       </c>
       <c r="G13" s="3"/>
@@ -1751,7 +1751,7 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>108</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1773,7 +1773,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>109</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1795,7 +1795,7 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>260</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1817,7 +1817,7 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>110</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1839,7 +1839,7 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <v>1.1599999999999999</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1848,10 +1848,10 @@
       <c r="D18" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>148</v>
       </c>
       <c r="G18" s="3"/>
@@ -1861,7 +1861,7 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>113</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1883,7 +1883,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>112</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1892,10 +1892,10 @@
       <c r="D20" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>156</v>
       </c>
       <c r="G20" s="3"/>
@@ -1905,7 +1905,7 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>111</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1927,7 +1927,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>115</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1949,7 +1949,7 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>116</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1958,10 +1958,10 @@
       <c r="D23" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="24" t="s">
         <v>22</v>
       </c>
       <c r="G23" s="3"/>
@@ -1971,7 +1971,7 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>123</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1993,7 +1993,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="11" t="s">
         <v>114</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -2015,7 +2015,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>126</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -2037,7 +2037,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>117</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2046,7 +2046,7 @@
       <c r="D27" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="23" t="s">
         <v>210</v>
       </c>
       <c r="F27" s="7" t="s">
@@ -2059,7 +2059,7 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>118</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2068,7 +2068,7 @@
       <c r="D28" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="23" t="s">
         <v>211</v>
       </c>
       <c r="F28" s="7" t="s">
@@ -2081,7 +2081,7 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>121</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -2090,7 +2090,7 @@
       <c r="D29" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="23" t="s">
         <v>212</v>
       </c>
       <c r="F29" s="7" t="s">
@@ -2103,7 +2103,7 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="11" t="s">
         <v>122</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -2112,7 +2112,7 @@
       <c r="D30" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="23" t="s">
         <v>163</v>
       </c>
       <c r="F30" s="7" t="s">
@@ -2125,10 +2125,10 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="11">
         <v>1.29</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="16" t="s">
         <v>74</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -2147,10 +2147,10 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="16" t="s">
         <v>74</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -2169,10 +2169,10 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="11">
         <v>1.31</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C33" s="16" t="s">
         <v>74</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -2191,10 +2191,10 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="11">
         <v>1.32</v>
       </c>
-      <c r="C34" s="17"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="3"/>
       <c r="E34" s="6" t="s">
         <v>141</v>
@@ -2209,7 +2209,7 @@
         <f>+A34+1</f>
         <v>33</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="11" t="s">
         <v>119</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -2231,7 +2231,7 @@
         <f>+A35+1</f>
         <v>34</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="11" t="s">
         <v>120</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -2253,10 +2253,10 @@
         <f t="shared" ref="A37:A60" si="1">+A36+1</f>
         <v>35</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="11">
         <v>1.35</v>
       </c>
-      <c r="C37" s="17"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="3"/>
       <c r="E37" s="6" t="s">
         <v>175</v>
@@ -2271,10 +2271,10 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="11">
         <v>1.36</v>
       </c>
-      <c r="C38" s="17"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="3"/>
       <c r="E38" s="6" t="s">
         <v>144</v>
@@ -2289,10 +2289,10 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B39" s="12">
+      <c r="B39" s="11">
         <v>1.37</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="16" t="s">
         <v>74</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -2311,16 +2311,16 @@
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B40" s="11">
         <v>1.38</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="16" t="s">
         <v>74</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="23" t="s">
         <v>216</v>
       </c>
       <c r="F40" s="7" t="s">
@@ -2333,16 +2333,16 @@
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="11">
         <v>1.39</v>
       </c>
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="16" t="s">
         <v>74</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="23" t="s">
         <v>164</v>
       </c>
       <c r="F41" s="7" t="s">
@@ -2355,19 +2355,19 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C42" s="17" t="s">
+      <c r="C42" s="16" t="s">
         <v>261</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E42" s="24" t="s">
+      <c r="E42" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="F42" s="25" t="s">
+      <c r="F42" s="24" t="s">
         <v>154</v>
       </c>
       <c r="G42" s="3"/>
@@ -2377,7 +2377,7 @@
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B43" s="11">
         <v>1.41</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2386,10 +2386,10 @@
       <c r="D43" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E43" s="24" t="s">
+      <c r="E43" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="F43" s="25" t="s">
+      <c r="F43" s="24" t="s">
         <v>11</v>
       </c>
       <c r="G43" s="3"/>
@@ -2399,7 +2399,7 @@
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B44" s="11">
         <v>1.42</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -2421,7 +2421,7 @@
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="B45" s="12">
+      <c r="B45" s="11">
         <v>1.43</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2430,7 +2430,7 @@
       <c r="D45" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E45" s="24" t="s">
+      <c r="E45" s="23" t="s">
         <v>218</v>
       </c>
       <c r="F45" s="7" t="s">
@@ -2439,20 +2439,20 @@
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="20">
+      <c r="A46" s="19">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="B46" s="21">
+      <c r="B46" s="20">
         <v>1.44</v>
       </c>
-      <c r="C46" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" s="20" t="s">
+      <c r="C46" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E46" s="23" t="s">
         <v>142</v>
       </c>
       <c r="F46" s="7" t="s">
@@ -2461,17 +2461,17 @@
       <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="20">
+      <c r="A47" s="19">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="B47" s="21">
+      <c r="B47" s="20">
         <v>1.45</v>
       </c>
-      <c r="C47" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D47" s="20" t="s">
+      <c r="C47" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="19" t="s">
         <v>82</v>
       </c>
       <c r="E47" s="6" t="s">
@@ -2483,20 +2483,20 @@
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="20">
+      <c r="A48" s="19">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="B48" s="21">
+      <c r="B48" s="20">
         <v>1.46</v>
       </c>
-      <c r="C48" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D48" s="20" t="s">
+      <c r="C48" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E48" s="24" t="s">
+      <c r="E48" s="23" t="s">
         <v>178</v>
       </c>
       <c r="F48" s="7" t="s">
@@ -2505,20 +2505,20 @@
       <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="20">
+      <c r="A49" s="19">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B49" s="21">
+      <c r="B49" s="20">
         <v>1.47</v>
       </c>
-      <c r="C49" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D49" s="20" t="s">
+      <c r="C49" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D49" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E49" s="24" t="s">
+      <c r="E49" s="23" t="s">
         <v>185</v>
       </c>
       <c r="F49" s="7" t="s">
@@ -2527,11 +2527,11 @@
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="20">
+      <c r="A50" s="19">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="11" t="s">
         <v>128</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -2540,20 +2540,20 @@
       <c r="D50" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E50" s="24" t="s">
+      <c r="E50" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="F50" s="25" t="s">
+      <c r="F50" s="24" t="s">
         <v>57</v>
       </c>
       <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="20">
+      <c r="A51" s="19">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="11" t="s">
         <v>129</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -2562,7 +2562,7 @@
       <c r="D51" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E51" s="24" t="s">
+      <c r="E51" s="23" t="s">
         <v>220</v>
       </c>
       <c r="F51" s="7" t="s">
@@ -2571,11 +2571,11 @@
       <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="20">
+      <c r="A52" s="19">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="11" t="s">
         <v>127</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -2584,20 +2584,20 @@
       <c r="D52" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E52" s="22" t="s">
+      <c r="E52" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="F52" s="11" t="s">
+      <c r="F52" s="10" t="s">
         <v>190</v>
       </c>
       <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="20">
+      <c r="A53" s="19">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="11" t="s">
         <v>262</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2615,11 +2615,11 @@
       <c r="G53" s="3"/>
     </row>
     <row r="54" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="20">
+      <c r="A54" s="19">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="11" t="s">
         <v>263</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -2628,20 +2628,20 @@
       <c r="D54" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E54" s="22" t="s">
+      <c r="E54" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F54" s="10" t="s">
         <v>174</v>
       </c>
       <c r="G54" s="3"/>
     </row>
     <row r="55" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="20">
+      <c r="A55" s="19">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="11" t="s">
         <v>264</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -2659,11 +2659,11 @@
       <c r="G55" s="3"/>
     </row>
     <row r="56" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="20">
+      <c r="A56" s="19">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="11" t="s">
         <v>265</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -2681,11 +2681,11 @@
       <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="20">
+      <c r="A57" s="19">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="B57" s="12">
+      <c r="B57" s="11">
         <v>1.55</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -2703,11 +2703,11 @@
       <c r="G57" s="3"/>
     </row>
     <row r="58" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="20">
+      <c r="A58" s="19">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="11" t="s">
         <v>267</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -2725,11 +2725,11 @@
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="20">
+      <c r="A59" s="19">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="B59" s="11" t="s">
         <v>266</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -2747,17 +2747,17 @@
       <c r="G59" s="3"/>
     </row>
     <row r="60" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="20">
+      <c r="A60" s="19">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="B60" s="21" t="s">
+      <c r="B60" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="C60" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D60" s="20" t="s">
+      <c r="C60" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60" s="19" t="s">
         <v>268</v>
       </c>
       <c r="E60" s="6" t="s">
@@ -2773,13 +2773,13 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B61" s="21">
+      <c r="B61" s="20">
         <v>1.59</v>
       </c>
-      <c r="C61" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D61" s="20" t="s">
+      <c r="C61" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61" s="19" t="s">
         <v>271</v>
       </c>
       <c r="E61" s="6" t="s">
@@ -2791,17 +2791,17 @@
       <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="20">
+      <c r="A62" s="19">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B62" s="21" t="s">
+      <c r="B62" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="C62" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="D62" s="20" t="s">
+      <c r="C62" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" s="19" t="s">
         <v>271</v>
       </c>
       <c r="E62" s="6" t="s">
@@ -2813,14 +2813,14 @@
       <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="20">
+      <c r="A63" s="19">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B63" s="21" t="s">
+      <c r="B63" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="C63" s="19" t="s">
         <v>74</v>
       </c>
       <c r="D63" s="3" t="s">
@@ -2835,14 +2835,14 @@
       <c r="G63" s="3"/>
     </row>
     <row r="64" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="20">
+      <c r="A64" s="19">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B64" s="21" t="s">
+      <c r="B64" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="19" t="s">
         <v>74</v>
       </c>
       <c r="D64" s="3" t="s">
@@ -2857,14 +2857,14 @@
       <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="20">
+      <c r="A65" s="19">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B65" s="21" t="s">
+      <c r="B65" s="20" t="s">
         <v>274</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="19" t="s">
         <v>74</v>
       </c>
       <c r="D65" s="3" t="s">
@@ -2879,14 +2879,14 @@
       <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="20">
+      <c r="A66" s="19">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B66" s="12">
+      <c r="B66" s="11">
         <v>1.64</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="19" t="s">
         <v>74</v>
       </c>
       <c r="D66" s="3" t="s">
@@ -2901,11 +2901,11 @@
       <c r="G66" s="3"/>
     </row>
     <row r="67" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="20">
+      <c r="A67" s="19">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B67" s="12">
+      <c r="B67" s="11">
         <v>1.65</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -2923,11 +2923,11 @@
       <c r="G67" s="3"/>
     </row>
     <row r="68" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="20">
+      <c r="A68" s="19">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B68" s="12">
+      <c r="B68" s="11">
         <v>1.66</v>
       </c>
       <c r="C68" s="3" t="s">
@@ -2936,20 +2936,20 @@
       <c r="D68" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="F68" s="10" t="s">
+      <c r="F68" s="7" t="s">
         <v>42</v>
       </c>
       <c r="G68" s="3"/>
     </row>
     <row r="69" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="20">
+      <c r="A69" s="19">
         <f t="shared" si="0"/>
         <v>67</v>
       </c>
-      <c r="B69" s="12">
+      <c r="B69" s="11">
         <v>1.67</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -2958,20 +2958,20 @@
       <c r="D69" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E69" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="F69" s="10" t="s">
+      <c r="F69" s="7" t="s">
         <v>39</v>
       </c>
       <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="20">
+      <c r="A70" s="19">
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="B70" s="12">
+      <c r="B70" s="11">
         <v>1.68</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -2983,17 +2983,17 @@
       <c r="E70" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="F70" s="10" t="s">
+      <c r="F70" s="7" t="s">
         <v>40</v>
       </c>
       <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="20">
+      <c r="A71" s="19">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="B71" s="12">
+      <c r="B71" s="11">
         <v>1.69</v>
       </c>
       <c r="C71" s="3" t="s">
@@ -3011,11 +3011,11 @@
       <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="20">
+      <c r="A72" s="19">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="B72" s="12" t="s">
+      <c r="B72" s="11" t="s">
         <v>280</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -3033,11 +3033,11 @@
       <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="20">
+      <c r="A73" s="19">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="B73" s="12">
+      <c r="B73" s="11">
         <v>1.71</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -3055,11 +3055,11 @@
       <c r="G73" s="3"/>
     </row>
     <row r="74" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="20">
+      <c r="A74" s="19">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="B74" s="12" t="s">
+      <c r="B74" s="11" t="s">
         <v>281</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -3077,11 +3077,11 @@
       <c r="G74" s="3"/>
     </row>
     <row r="75" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="20">
+      <c r="A75" s="19">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
-      <c r="B75" s="12" t="s">
+      <c r="B75" s="11" t="s">
         <v>282</v>
       </c>
       <c r="C75" s="3" t="s">
@@ -3090,7 +3090,7 @@
       <c r="D75" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E75" s="24" t="s">
+      <c r="E75" s="23" t="s">
         <v>230</v>
       </c>
       <c r="F75" s="7" t="s">
@@ -3099,11 +3099,11 @@
       <c r="G75" s="3"/>
     </row>
     <row r="76" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="20">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="B76" s="12">
+      <c r="A76" s="19">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="B76" s="11">
         <v>1.74</v>
       </c>
       <c r="C76" s="3" t="s">
@@ -3112,7 +3112,7 @@
       <c r="D76" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E76" s="24" t="s">
+      <c r="E76" s="23" t="s">
         <v>231</v>
       </c>
       <c r="F76" s="7" t="s">
@@ -3121,11 +3121,11 @@
       <c r="G76" s="3"/>
     </row>
     <row r="77" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="20">
+      <c r="A77" s="19">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="B77" s="12" t="s">
+      <c r="B77" s="11" t="s">
         <v>283</v>
       </c>
       <c r="C77" s="3" t="s">
@@ -3143,11 +3143,11 @@
       <c r="G77" s="3"/>
     </row>
     <row r="78" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="20">
+      <c r="A78" s="19">
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="B78" s="12" t="s">
+      <c r="B78" s="11" t="s">
         <v>284</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -3156,7 +3156,7 @@
       <c r="D78" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E78" s="24" t="s">
+      <c r="E78" s="23" t="s">
         <v>233</v>
       </c>
       <c r="F78" s="7" t="s">
@@ -3165,11 +3165,11 @@
       <c r="G78" s="3"/>
     </row>
     <row r="79" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="20">
+      <c r="A79" s="19">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="B79" s="12" t="s">
+      <c r="B79" s="11" t="s">
         <v>285</v>
       </c>
       <c r="C79" s="3" t="s">
@@ -3178,7 +3178,7 @@
       <c r="D79" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E79" s="24" t="s">
+      <c r="E79" s="23" t="s">
         <v>235</v>
       </c>
       <c r="F79" s="7" t="s">
@@ -3187,11 +3187,11 @@
       <c r="G79" s="3"/>
     </row>
     <row r="80" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="20">
+      <c r="A80" s="19">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="11" t="s">
         <v>286</v>
       </c>
       <c r="C80" s="3" t="s">
@@ -3209,11 +3209,11 @@
       <c r="G80" s="3"/>
     </row>
     <row r="81" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="20">
+      <c r="A81" s="19">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="B81" s="12">
+      <c r="B81" s="11">
         <v>1.79</v>
       </c>
       <c r="C81" s="3" t="s">
@@ -3231,17 +3231,17 @@
       <c r="G81" s="3"/>
     </row>
     <row r="82" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="20">
+      <c r="A82" s="19">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="B82" s="12">
+      <c r="B82" s="11">
         <v>1.8</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D82" s="19"/>
+      <c r="D82" s="18"/>
       <c r="E82" s="6" t="s">
         <v>165</v>
       </c>
@@ -3251,17 +3251,17 @@
       <c r="G82" s="3"/>
     </row>
     <row r="83" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="20">
+      <c r="A83" s="19">
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="B83" s="12">
+      <c r="B83" s="11">
         <v>1.81</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D83" s="19"/>
+      <c r="D83" s="18"/>
       <c r="E83" s="6" t="s">
         <v>191</v>
       </c>
@@ -3271,11 +3271,11 @@
       <c r="G83" s="3"/>
     </row>
     <row r="84" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="20">
+      <c r="A84" s="19">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="B84" s="12" t="s">
+      <c r="B84" s="11" t="s">
         <v>133</v>
       </c>
       <c r="C84" s="3" t="s">
@@ -3293,11 +3293,11 @@
       <c r="G84" s="3"/>
     </row>
     <row r="85" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="20">
+      <c r="A85" s="19">
         <f t="shared" si="0"/>
         <v>83</v>
       </c>
-      <c r="B85" s="12">
+      <c r="B85" s="11">
         <v>2.2000000000000002</v>
       </c>
       <c r="C85" s="3" t="s">
@@ -3315,11 +3315,11 @@
       <c r="G85" s="3"/>
     </row>
     <row r="86" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="20">
+      <c r="A86" s="19">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="B86" s="12">
+      <c r="B86" s="11">
         <v>2.2999999999999998</v>
       </c>
       <c r="C86" s="3" t="s">
@@ -3328,7 +3328,7 @@
       <c r="D86" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E86" s="24" t="s">
+      <c r="E86" s="23" t="s">
         <v>234</v>
       </c>
       <c r="F86" s="7" t="s">
@@ -3337,11 +3337,11 @@
       <c r="G86" s="3"/>
     </row>
     <row r="87" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="20">
+      <c r="A87" s="19">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="B87" s="12">
+      <c r="B87" s="11">
         <v>2.4</v>
       </c>
       <c r="C87" s="3" t="s">
@@ -3359,11 +3359,11 @@
       <c r="G87" s="3"/>
     </row>
     <row r="88" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="20">
+      <c r="A88" s="19">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
-      <c r="B88" s="12">
+      <c r="B88" s="11">
         <v>2.5</v>
       </c>
       <c r="C88" s="3" t="s">
@@ -3381,11 +3381,11 @@
       <c r="G88" s="3"/>
     </row>
     <row r="89" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="20">
+      <c r="A89" s="19">
         <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="B89" s="12">
+      <c r="B89" s="11">
         <v>2.6</v>
       </c>
       <c r="C89" s="3" t="s">
@@ -3394,7 +3394,7 @@
       <c r="D89" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E89" s="24" t="s">
+      <c r="E89" s="23" t="s">
         <v>241</v>
       </c>
       <c r="F89" s="7" t="s">
@@ -3403,11 +3403,11 @@
       <c r="G89" s="3"/>
     </row>
     <row r="90" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="20">
+      <c r="A90" s="19">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="B90" s="12">
+      <c r="B90" s="11">
         <v>2.7</v>
       </c>
       <c r="C90" s="3" t="s">
@@ -3416,7 +3416,7 @@
       <c r="D90" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E90" s="24" t="s">
+      <c r="E90" s="23" t="s">
         <v>241</v>
       </c>
       <c r="F90" s="7" t="s">
@@ -3425,11 +3425,11 @@
       <c r="G90" s="3"/>
     </row>
     <row r="91" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="20">
+      <c r="A91" s="19">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="B91" s="12">
+      <c r="B91" s="11">
         <v>2.8</v>
       </c>
       <c r="C91" s="3" t="s">
@@ -3447,11 +3447,11 @@
       <c r="G91" s="3"/>
     </row>
     <row r="92" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="20">
+      <c r="A92" s="19">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="B92" s="12">
+      <c r="B92" s="11">
         <v>2.9</v>
       </c>
       <c r="C92" s="3" t="s">
@@ -3469,11 +3469,11 @@
       <c r="G92" s="3"/>
     </row>
     <row r="93" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="20">
+      <c r="A93" s="19">
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="B93" s="12" t="s">
+      <c r="B93" s="11" t="s">
         <v>102</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -3482,20 +3482,20 @@
       <c r="D93" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E93" s="24" t="s">
+      <c r="E93" s="23" t="s">
         <v>244</v>
       </c>
-      <c r="F93" s="25" t="s">
+      <c r="F93" s="24" t="s">
         <v>18</v>
       </c>
       <c r="G93" s="3"/>
     </row>
     <row r="94" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="20">
+      <c r="A94" s="19">
         <f t="shared" si="0"/>
         <v>92</v>
       </c>
-      <c r="B94" s="12" t="s">
+      <c r="B94" s="11" t="s">
         <v>131</v>
       </c>
       <c r="C94" s="3" t="s">
@@ -3513,11 +3513,11 @@
       <c r="G94" s="3"/>
     </row>
     <row r="95" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="20">
+      <c r="A95" s="19">
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="B95" s="12">
+      <c r="B95" s="11">
         <v>2.12</v>
       </c>
       <c r="C95" s="3" t="s">
@@ -3535,11 +3535,11 @@
       <c r="G95" s="3"/>
     </row>
     <row r="96" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="20">
+      <c r="A96" s="19">
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
-      <c r="B96" s="12" t="s">
+      <c r="B96" s="11" t="s">
         <v>132</v>
       </c>
       <c r="C96" s="3" t="s">
@@ -3548,7 +3548,7 @@
       <c r="D96" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E96" s="24" t="s">
+      <c r="E96" s="23" t="s">
         <v>246</v>
       </c>
       <c r="F96" s="7" t="s">
@@ -3557,11 +3557,11 @@
       <c r="G96" s="3"/>
     </row>
     <row r="97" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="20">
+      <c r="A97" s="19">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="B97" s="12" t="s">
+      <c r="B97" s="11" t="s">
         <v>130</v>
       </c>
       <c r="C97" s="3" t="s">
@@ -3570,20 +3570,20 @@
       <c r="D97" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E97" s="24" t="s">
+      <c r="E97" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="F97" s="25" t="s">
+      <c r="F97" s="24" t="s">
         <v>20</v>
       </c>
       <c r="G97" s="3"/>
     </row>
     <row r="98" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="20">
+      <c r="A98" s="19">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="B98" s="12">
+      <c r="B98" s="11">
         <v>2.15</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -3592,20 +3592,20 @@
       <c r="D98" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E98" s="24" t="s">
+      <c r="E98" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="F98" s="25" t="s">
+      <c r="F98" s="24" t="s">
         <v>21</v>
       </c>
       <c r="G98" s="3"/>
     </row>
     <row r="99" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="20">
+      <c r="A99" s="19">
         <f t="shared" si="0"/>
         <v>97</v>
       </c>
-      <c r="B99" s="14" t="s">
+      <c r="B99" s="13" t="s">
         <v>134</v>
       </c>
       <c r="C99" s="3" t="s">
@@ -3623,11 +3623,11 @@
       <c r="G99" s="3"/>
     </row>
     <row r="100" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="20">
+      <c r="A100" s="19">
         <f t="shared" si="0"/>
         <v>98</v>
       </c>
-      <c r="B100" s="12" t="s">
+      <c r="B100" s="11" t="s">
         <v>135</v>
       </c>
       <c r="C100" s="3" t="s">
@@ -3636,7 +3636,7 @@
       <c r="D100" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E100" s="23" t="s">
+      <c r="E100" s="22" t="s">
         <v>249</v>
       </c>
       <c r="F100" s="7" t="s">
@@ -3645,11 +3645,11 @@
       <c r="G100" s="3"/>
     </row>
     <row r="101" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="20">
+      <c r="A101" s="19">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="B101" s="12" t="s">
+      <c r="B101" s="11" t="s">
         <v>136</v>
       </c>
       <c r="C101" s="3" t="s">
@@ -3658,7 +3658,7 @@
       <c r="D101" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E101" s="24" t="s">
+      <c r="E101" s="23" t="s">
         <v>248</v>
       </c>
       <c r="F101" s="7" t="s">
@@ -3667,11 +3667,11 @@
       <c r="G101" s="3"/>
     </row>
     <row r="102" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="20">
+      <c r="A102" s="19">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="B102" s="12" t="s">
+      <c r="B102" s="11" t="s">
         <v>137</v>
       </c>
       <c r="C102" s="3" t="s">
@@ -3689,11 +3689,11 @@
       <c r="G102" s="3"/>
     </row>
     <row r="103" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="20">
+      <c r="A103" s="19">
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="B103" s="12" t="s">
+      <c r="B103" s="11" t="s">
         <v>291</v>
       </c>
       <c r="C103" s="3" t="s">
@@ -3711,11 +3711,11 @@
       <c r="G103" s="3"/>
     </row>
     <row r="104" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="20">
+      <c r="A104" s="19">
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="B104" s="12" t="s">
+      <c r="B104" s="11" t="s">
         <v>290</v>
       </c>
       <c r="C104" s="3" t="s">
@@ -3733,11 +3733,11 @@
       <c r="G104" s="3"/>
     </row>
     <row r="105" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="20">
+      <c r="A105" s="19">
         <f t="shared" si="0"/>
         <v>103</v>
       </c>
-      <c r="B105" s="12" t="s">
+      <c r="B105" s="11" t="s">
         <v>292</v>
       </c>
       <c r="C105" s="3" t="s">
@@ -3755,11 +3755,11 @@
       <c r="G105" s="3"/>
     </row>
     <row r="106" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="20">
+      <c r="A106" s="19">
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-      <c r="B106" s="12" t="s">
+      <c r="B106" s="11" t="s">
         <v>293</v>
       </c>
       <c r="C106" s="3" t="s">
@@ -3777,11 +3777,11 @@
       <c r="G106" s="3"/>
     </row>
     <row r="107" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="20">
+      <c r="A107" s="19">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="B107" s="12">
+      <c r="B107" s="11">
         <v>2.2400000000000002</v>
       </c>
       <c r="C107" s="3" t="s">
@@ -3790,20 +3790,20 @@
       <c r="D107" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E107" s="24" t="s">
+      <c r="E107" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="F107" s="25" t="s">
+      <c r="F107" s="24" t="s">
         <v>5</v>
       </c>
       <c r="G107" s="3"/>
     </row>
     <row r="108" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="20">
+      <c r="A108" s="19">
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
-      <c r="B108" s="12" t="s">
+      <c r="B108" s="11" t="s">
         <v>294</v>
       </c>
       <c r="C108" s="3" t="s">
@@ -3812,7 +3812,7 @@
       <c r="D108" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E108" s="24" t="s">
+      <c r="E108" s="23" t="s">
         <v>252</v>
       </c>
       <c r="F108" s="7" t="s">
@@ -3821,11 +3821,11 @@
       <c r="G108" s="3"/>
     </row>
     <row r="109" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="20">
+      <c r="A109" s="19">
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="B109" s="12">
+      <c r="B109" s="11">
         <v>2.2599999999999998</v>
       </c>
       <c r="C109" s="3" t="s">
@@ -3843,11 +3843,11 @@
       <c r="G109" s="3"/>
     </row>
     <row r="110" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="20">
+      <c r="A110" s="19">
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
-      <c r="B110" s="12">
+      <c r="B110" s="11">
         <v>2.27</v>
       </c>
       <c r="C110" s="3" t="s">
@@ -3866,79 +3866,79 @@
     </row>
     <row r="111" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
-      <c r="B111" s="18"/>
-      <c r="C111" s="19"/>
-      <c r="D111" s="19"/>
-      <c r="E111" s="19"/>
-      <c r="F111" s="19"/>
+      <c r="B111" s="17"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="18"/>
+      <c r="F111" s="18"/>
       <c r="G111" s="3"/>
     </row>
     <row r="112" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
-      <c r="B112" s="18"/>
-      <c r="C112" s="19"/>
-      <c r="D112" s="19"/>
-      <c r="E112" s="19"/>
-      <c r="F112" s="19"/>
+      <c r="B112" s="17"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="18"/>
+      <c r="F112" s="18"/>
       <c r="G112" s="3"/>
     </row>
     <row r="113" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
-      <c r="B113" s="18"/>
-      <c r="C113" s="19"/>
-      <c r="D113" s="19"/>
-      <c r="E113" s="19"/>
-      <c r="F113" s="19"/>
+      <c r="B113" s="17"/>
+      <c r="C113" s="18"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="18"/>
+      <c r="F113" s="18"/>
       <c r="G113" s="3"/>
     </row>
     <row r="114" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
-      <c r="B114" s="18"/>
-      <c r="C114" s="19"/>
-      <c r="D114" s="19"/>
-      <c r="E114" s="19"/>
-      <c r="F114" s="19"/>
+      <c r="B114" s="17"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="18"/>
+      <c r="F114" s="18"/>
       <c r="G114" s="3"/>
     </row>
     <row r="115" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
-      <c r="B115" s="18"/>
-      <c r="C115" s="19"/>
-      <c r="D115" s="19"/>
-      <c r="E115" s="19"/>
-      <c r="F115" s="19"/>
+      <c r="B115" s="17"/>
+      <c r="C115" s="18"/>
+      <c r="D115" s="18"/>
+      <c r="E115" s="18"/>
+      <c r="F115" s="18"/>
       <c r="G115" s="3"/>
     </row>
     <row r="116" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
-      <c r="B116" s="18"/>
-      <c r="C116" s="19"/>
-      <c r="D116" s="19"/>
-      <c r="E116" s="19"/>
-      <c r="F116" s="19"/>
+      <c r="B116" s="17"/>
+      <c r="C116" s="18"/>
+      <c r="D116" s="18"/>
+      <c r="E116" s="18"/>
+      <c r="F116" s="18"/>
       <c r="G116" s="3"/>
     </row>
     <row r="117" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
-      <c r="B117" s="18"/>
-      <c r="C117" s="19"/>
-      <c r="D117" s="19"/>
-      <c r="E117" s="19"/>
-      <c r="F117" s="19"/>
+      <c r="B117" s="17"/>
+      <c r="C117" s="18"/>
+      <c r="D117" s="18"/>
+      <c r="E117" s="18"/>
+      <c r="F117" s="18"/>
       <c r="G117" s="3"/>
     </row>
     <row r="118" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
-      <c r="B118" s="18"/>
-      <c r="C118" s="19"/>
-      <c r="D118" s="19"/>
-      <c r="E118" s="19"/>
-      <c r="F118" s="19"/>
+      <c r="B118" s="17"/>
+      <c r="C118" s="18"/>
+      <c r="D118" s="18"/>
+      <c r="E118" s="18"/>
+      <c r="F118" s="18"/>
       <c r="G118" s="3"/>
     </row>
     <row r="119" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
-      <c r="B119" s="15"/>
+      <c r="B119" s="14"/>
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>

</xml_diff>